<commit_message>
Adding Antigen Test fields
Signed-off-by: Vitor Pamplona <vitor@vitorpamplona.com>
</commit_message>
<xml_diff>
--- a/examples/GHP_data_capture_CA_draft.xlsx
+++ b/examples/GHP_data_capture_CA_draft.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pknowles/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DCC7284-9A49-1842-AF9F-65956CEA832D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917828DB-F94F-5F42-B188-4D789022563A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1160" yWindow="500" windowWidth="24780" windowHeight="16340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="READ ME" sheetId="15" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="308">
   <si>
     <t>Text</t>
   </si>
@@ -692,30 +692,6 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Format Overlay</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t> is a core linked object that defines attribute formats, field lengths, or dictionary coding schemes (e.g., YYYY-MM-DD, SNOMED CT, ISO 3166-1 alpha-2, etc.).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>A </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
       <t>Meta Overlay</t>
     </r>
     <r>
@@ -917,10 +893,6 @@
     <t>CA:Canada (le)</t>
   </si>
   <si>
-    <t xml:space="preserve">Vaccination Credential
-</t>
-  </si>
-  <si>
     <t>SAI = Self-Addressing Identifier</t>
   </si>
   <si>
@@ -980,15 +952,6 @@
   </si>
   <si>
     <t>CVX</t>
-  </si>
-  <si>
-    <t>MOD:Moderna US, Inc.|PFR:Pfizer, Inc|ASZ:AstraZeneca|JSN:Janssen</t>
-  </si>
-  <si>
-    <t>MVX</t>
-  </si>
-  <si>
-    <t>MOD|PFR|ASZ|JSN</t>
   </si>
   <si>
     <t>207|208|210|212</t>
@@ -1075,6 +1038,305 @@
       </rPr>
       <t> is a stable base object that defines a single data set in its purest form, thus providing a standard base to decentralise data. The construct also contains a flagging block, which allows the issuer to flag any attributes that could potentially unblind the identity of a governing entity. With identifying attributes flagged at the base layer, all corresponding data can be treated as sensitive throughout a data lifecycle and encrypted or removed at any stage, thus reducing the risk of identifying governing entities in blinded datasets.</t>
     </r>
+  </si>
+  <si>
+    <t>Entry Codes Overlay</t>
+  </si>
+  <si>
+    <r>
+      <t>A </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Format Overla</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>y is a core linked object that defines attribute formats, field lengths, or dictionary coding schemes (e.g., YYYY-MM-DD, SNOMED CT, ISO 3166-1 alpha-2, etc.).</t>
+    </r>
+  </si>
+  <si>
+    <t>linkedTestCertificate</t>
+  </si>
+  <si>
+    <t>DRI</t>
+  </si>
+  <si>
+    <t>testType</t>
+  </si>
+  <si>
+    <t>LOINC</t>
+  </si>
+  <si>
+    <t>testCommercialName</t>
+  </si>
+  <si>
+    <t>testManufacturer</t>
+  </si>
+  <si>
+    <t>dateOfSample</t>
+  </si>
+  <si>
+    <t>YYYY-MM-DDThh:mm:ssZ</t>
+  </si>
+  <si>
+    <t>dateOfResult</t>
+  </si>
+  <si>
+    <t>testResult</t>
+  </si>
+  <si>
+    <t>testingCentre</t>
+  </si>
+  <si>
+    <t>stateOfTest</t>
+  </si>
+  <si>
+    <t>countryOfTest</t>
+  </si>
+  <si>
+    <t>COVID-19 Antigen Test Credential</t>
+  </si>
+  <si>
+    <t>A form to be used for verifiable COVID-19 antigen test credentials for basic interoperability</t>
+  </si>
+  <si>
+    <t>Personal/Operational|Linked test certificate ID</t>
+  </si>
+  <si>
+    <t>Unique identifier of the associated test certificate</t>
+  </si>
+  <si>
+    <t>Test information|Disease or agent targeted|Classification of Disease</t>
+  </si>
+  <si>
+    <t>Disease or agent that the test provides detection of.</t>
+  </si>
+  <si>
+    <t>Description of the type of test that was conducted, e.g. NAAT or rapid antigen test.</t>
+  </si>
+  <si>
+    <t>Commercial or brand name of the test.</t>
+  </si>
+  <si>
+    <t>Test information|Test manufacturer</t>
+  </si>
+  <si>
+    <t>Legal manufacturer of the test.</t>
+  </si>
+  <si>
+    <t>Test information|Date and time of the test sample collection</t>
+  </si>
+  <si>
+    <t>Date and time when the sample was collected.</t>
+  </si>
+  <si>
+    <t>Test information|Date and time of the test result production</t>
+  </si>
+  <si>
+    <t>Date and time when the test result was produced.</t>
+  </si>
+  <si>
+    <t>Test information|Result of the test</t>
+  </si>
+  <si>
+    <t>For example, negative, positive, inconclusive or void.</t>
+  </si>
+  <si>
+    <t>Test information|Testing centre or facility</t>
+  </si>
+  <si>
+    <t>Name/code of testing centre, facility or a health authority responsible for the testing event.</t>
+  </si>
+  <si>
+    <t>Test information|Province or territory where the test was taken</t>
+  </si>
+  <si>
+    <t>The province or territory in which the individual was tested</t>
+  </si>
+  <si>
+    <t>Test information|Country where the test was taken</t>
+  </si>
+  <si>
+    <t>The country in which the individual was tested.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LP6464-4|LP217198-3 </t>
+  </si>
+  <si>
+    <t>260415000|260373001</t>
+  </si>
+  <si>
+    <t>260415000:Not detected|260373001:Detected</t>
+  </si>
+  <si>
+    <t>LP6464-4:Nucleic acid amplification with probe detection|LP217198-3:Rapid immunoassay</t>
+  </si>
+  <si>
+    <t>Test information|Test commercial name</t>
+  </si>
+  <si>
+    <t>GLN-8800075500014|GLN-0811877010005|GLN-0813337010006|GLN-0884999000001|GLN-4051892000001|LEI-549300883RE115J3LD19|CRN-2354710|GLN-0382900000008|DUNS-962942756|GLN-0851458005006|GLN-0815381020000|GLN-0860004739708|GLN-3015730200108|GLN-3610520000007|DUNS-251005005|DUNS-956711444|GLN-0810040820007|CRN-103082|GLN-0014613000005|DUNS-033429783|GLN-0816101020003|GLN-0893230002001|GLN-4049016000006|GLN-5453003370000|DUNS-153623137|GLN-5060887160001|GLN-0816270020002|DUNS-004006628|DUNS-243942278|GLN-0850021628000|GLN-0810055970001|GLN-0840487100004|DUNS-255371916|CRN-842762684|GLN-4065384000004|CRN-330215000039151|LEI-549300ZZX9WCBZNYL849|GLN-0758750000008|GLN-0885502000006|GLN-8800047500011|GLN-4053228000006|GLN-0014613000005|GLN-0812589020009|CRN-743768921|GLN-4038377000008|GLN-0875197000009|DUNS-421167832|GLN-8800111700019|GLN-8800069800014|GLN-8809240100011|CRN-310115000888557|GLN-0842768000003|GLN-8809517360018|DUNS-243605917|GLN-0850000184008|CRN-350200200037950</t>
+  </si>
+  <si>
+    <t>GLN-8800075500014:1drop Inc. (South Korea)|GLN-0811877010005:Abbott Diagnostics Scarborough, Inc. (United States)|GLN-0813337010006:Abbott Laboratories Diagnostics Division (United States)|GLN-0884999000001:Abbott Molecular Inc. (United States)|GLN-4051892000001:Abbott Rapid Diagnostics Jena Gmbh (Germany)|LEI-549300883RE115J3LD19:Artron Laboratories Inc. (Canada)|CRN-2354710:Assure Tech. (Hangzhou) Co. Ltd. (China)|GLN-0382900000008:Becton Dickinson And Company (Bd) (United States)|DUNS-962942756:Bgi Americas Corp (United States)|GLN-0851458005006:Biofire Defense (United States)|GLN-0815381020000:Biofire Diagnostics, Llc. (United States)|GLN-0860004739708:Biomeme Inc (United States)|GLN-3015730200108:Biomerieux Sa (France)|GLN-3610520000007:Bio-Rad (France)|DUNS-251005005:Btnx Inc. (Canada)|DUNS-956711444:Cepheid (United States)|GLN-0810040820007:Cue Health Inc. (United States)|CRN-103082:Diagnostics Biochem Canada Inc. (Canada)|GLN-0014613000005:Diagnostic Hybrids, Inc. - Also Trading As Quidel Corporation (United States)|DUNS-033429783:Diasorin Inc. (United States)|GLN-0816101020003:Diasorin Molecular Llc (United States)|GLN-0893230002001:Epitope Diagnostics, Inc. (United States)|GLN-4049016000006:Euroimmun Medizinische Labordiagnostika Ag (Germany)|GLN-5453003370000:Fast Track Diagnostics Luxembourg S.A.R.L. (Luxembourg)|DUNS-153623137:Hologic, Inc. (United States)|GLN-5060887160001:Hyris Ltd (Great Britain)|GLN-0816270020002:Illumina, Inc. (United States)|DUNS-004006628:Inbios International Inc. (United States)|DUNS-243942278:International Point Of Care, Inc. (Canada)|GLN-0850021628000:Kantaro Biosciences, Llc (United States)|GLN-0810055970001:Lucira Health, Inc. (United States)|GLN-0840487100004:Luminex Corporation (United States)|DUNS-255371916:Luminex Molecular Diagnostics, Inc. (Canada)|CRN-842762684:Luminultra Technologies Ltd. (Canada)|GLN-4065384000004:Nal Von Minden Gmbh (Germany)|CRN-330215000039151:Ningbo Health Gene Technologies Co., Ltd (China)|LEI-549300ZZX9WCBZNYL849:Ortho-Clinical Diagnostics (Great Britain)|GLN-0758750000008:Ortho-Clinical Diagnostics Inc. (United States)|GLN-0885502000006:Osang Healthcare Co., Ltd. (South Korea)|GLN-8800047500011:Pcl Inc. (South Korea)|GLN-4053228000006:Qiagen Gmbh (Germany)|GLN-0014613000005:Quidel Corporation (United States)|GLN-0812589020009:Perkinelmer, Inc. (United States)|CRN-743768921:Precision Biomonitoring Inc. (Canada)|GLN-4038377000008:Roche Diagnostics Gmbh (Germany)|GLN-0875197000009:Roche Molecular Systems, Inc (United States)|DUNS-421167832:Sansure Biotech Inc. (China)|GLN-8800111700019:Sd Biosensor, Inc. (South Korea)|GLN-8800069800014:Seasun Biomaterials Inc. (South Korea)|GLN-8809240100011:Seegene Inc. (South Korea)|CRN-310115000888557:Shanghai Zj Bio-Tech Co., Ltd (China)|GLN-0842768000003:Siemens Healthcare Diagnostics Inc. (United States)|GLN-8809517360018:Solgent Co., Ltd. (South Korea)|DUNS-243605917:Spartan Bioscience Inc. (Canada)|GLN-0850000184008:Thermo Fisher Scientific (United States)|CRN-350200200037950:Xiamen Boson Biotech Co., Ltd. (China)</t>
+  </si>
+  <si>
+    <t>GLN-8800075500014/M22MD100M:1copy COVID-19 QPCR Multi Kit|GLN-0811877010005/190-080:Id Now COVID-19 Control Swab Kit|GLN-0811877010005/191-000:Id Now COVID-19|GLN-0813337010006/06R8601:SARS-CoV-2 IgG Calibrator Kit|GLN-0813337010006/06R8610:SARS-CoV-2 IgG Control Kit|GLN-0813337010006/06R8620:SARS-CoV-2 IgG Reagent Kit|GLN-0813337010006/06R8630:SARS-CoV-2 IgG Reagent Kit|GLN-0813337010006/06R9001:SARS-CoV-2 IgG Calibrator Kit|GLN-0813337010006/06R9010:SARS-CoV-2 IgG Control Kit|GLN-0813337010006/06R9020:SARS-CoV-2 IgG Reagent Kit|GLN-0813337010006/06R9030:SARS-CoV-2 IgG Reagent Kit|GLN-0884999000001/09N77-001:ABbott Realtime SARS-CoV-2 Application Cd-rom|GLN-0884999000001/09N77-010:ABbott Realtime SARS-CoV-2 Application Cd-rom|GLN-0884999000001/09N77-080:ABbott Realtime SARS-CoV-2 Control Kit|GLN-0884999000001/09N77-085:ABbott Realtime SARS-CoV-2 Control Kit|GLN-0884999000001/09N77-090:ABbott Realtime SARS-CoV-2 Amplification Reagent Kit|GLN-0884999000001/09N77-095:ABbott Realtime SARS-CoV-2 Amplification Reagent Kit|GLN-0884999000001/09N78-080:Alinity M SARS-CoV-2 Ctrl Kit|GLN-0884999000001/09N78-090:Alinity M SARS-CoV-2 Amp Kit|GLN-0884999000001/09N79-080:Alinity M Resp-4-plex Ctrl Kit|GLN-0884999000001/09N79-090:Alinity M Resp-4-plex Amp Kit|GLN-4051892000001/41FK10:Panbio COVID-19 AG Rapid Test Device (nasopharyngeal)|GLN-4051892000001/41FK11:Panbio COVID-19 AG Rapid Test Device (nasal)|LEI-549300883RE115J3LD19/A03-51-322:COVID-19 IgM/IgG Antibody Test|CRN-2354710/COV-W23M:COVID-19 IgG/IgM Rapid Test Device|GLN-0382900000008/256082:Bd Veritor System For Rapid Detection Of SARS-CoV-2|GLN-0382900000008/256089:Bd Veritor System For Rapid Detection Of SARS-CoV-2|GLN-0382900000008/445003-01:Bd SARS-CoV-2 Reagents For Bd Max System|DUNS-962942756/MFG030018:Real-time Fluorescent Rt-PCR Kit For Detecting SARS-CoV-2|GLN-0851458005006/423744:Biofire COVID-19 Test|GLN-0851458005006/423748:Biofire COVID-19 Test External Control Kit (+)|GLN-0815381020000/423738:Filmarray Respiratory Panel 2.1 (rp2.1)|GLN-0860004739708/1000003:Biomeme Franklin Three9 Real-time PCR Thermocycler|GLN-0860004739708/1000012:Rugged Android Smartphone W/ Biomeme Go Mobile App|GLN-0860004739708/1000013:Android Smartphone W/ Biomeme Go Mobile App|GLN-0860004739708/1000018:Biomeme Franklin Three9 Real-time PCR Thermocycler|GLN-0860004739708/3000011:Biomeme Fixed Volume Pipette Kit|GLN-0860004739708/3000150:Self-standing Tubes Pack|GLN-0860004739708/3000536:Biomeme M1 Sample Prep Cartridge Kit For Rna 2.0|GLN-0860004739708/3000555:Biomeme SARS-CoV-2 Go-strips|GLN-0860004739708/3000562:Biomeme SARS-CoV-2 Go-plates|GLN-0860004739708/3000563:Biomeme Sample Preparation Tray|GLN-0860004739708/3000564:Biomeme SARS-CoV-2 Bulk Vials|GLN-0860004739708/3000567:Transfer Pipette Pack|GLN-3015730200108/423720:Argene SARS-CoV-2 R-gene|GLN-3610520000007/72710:Platelia SARS-CoV-2 Total AB|GLN-3610520000007/12013798:Platelia SARS-CoV-2 Total AB|DUNS-251005005/COV-13C25:Rapid Response COVID-19 IgG/IgM Rapid Test Device|DUNS-956711444/XPCOV2/FLU/RSV-10:Xpert Xpress SARS-CoV-2/flu/RSV|DUNS-956711444/XPRSARS-COV2-10:Xpertxpress SARS-CoV-2|GLN-0810040820007/C0200:Cue Wireless Charging Base|GLN-0810040820007/C0201:Cue Health Monitoring System|GLN-0810040820007/C1021-01:Cue COVID-19 Test Cartridge Pack|GLN-0810040820007/C1021-03:Cue COVID-19 Test Cartridge Pack|GLN-0810040820007/C1021-10:Cue COVID-19 Test Cartridge Pack|GLN-0810040820007/C1021-100:Cue COVID-19 Test Cartridge Pack|GLN-0810040820007/C2113:Cue COVID-19 Test External Control Swabs Pack|GLN-0810040820007/CUE HEALTH APP:Cue Health Mobile Application|CRN-103082/CAN-IGG-19:Anti-SARS-CoV-2 IgG Elisa Kit|CRN-103082/CAN-IGT-19:Anti-SARS-CoV-2 Total Antibody (ab) Elisa Kit|GLN-0014613000005/M120:Lyra SARS-CoV-2 Assay|GLN-0014613000005/M124:Lyra Direct SARS-CoV-2 Assay|GLN-0014613000005/M313:Solana SARS-CoV-2 Assay|DUNS-033429783/311460:Liaison SARS-CoV-2 S1/s2 IgG|DUNS-033429783/311461:Liaison Control SARS-CoV-2 S1/s2 IgG|GLN-0816101020003/MOL4150:Simplexa COVID-19 Direct Assay|GLN-0816101020003/MOL4160:Simplexa COVID-19 Positive Control Pack|GLN-0893230002001/KT-1032:Edi Novel Coronavirus COVID-19 IgG Elisa Kit|GLN-4049016000006/EI 2606-9601 G:Anti-SARS-CoV-2 Elisa (IgG)|GLN-4049016000006/MP 2606-0100:Eurorealtime SARS-CoV-2|GLN-4049016000006/MP 2606-0125:Eurorealtime SARS-CoV-2|GLN-4049016000006/MP 2606-0200:Eurorealtime SARS-CoV-2|GLN-4049016000006/MP 2606-0225:Eurorealtime SARS-CoV-2|GLN-4049016000006/MP 2606-0425:Eurorealtime SARS-CoV-2|GLN-4049016000006/MP 2606-1000:Eurorealtime SARS-CoV-2|GLN-5453003370000/11416302 (FTD-114-96):Ftd SARS-CoV-2|DUNS-153623137/PRD-03546:Aptima Multitest Swab Specimen Collection Kit For SARS-CoV-2 Specimen Collection|DUNS-153623137/PRD-04303:Panther Fusion Open Access Rna/dna Enzyme Reagent Cartridge|DUNS-153623137/PRD-04304:Aptiman Oil Reagent Kit|DUNS-153623137/PRD-04331:Panther Fusion SARS-CoV-2 Extraction Reagent-s|DUNS-153623137/PRD-04332:Panther Fusion SARS-CoV-2 Internal Control-s|DUNS-153623137/PRD-04334:Panther Fusion SARS-CoV-2 Elution Buffer|DUNS-153623137/PRD-04335:Panther Fusion Oil|DUNS-153623137/PRD-06391:Panther Fusion SARS-CoV-2 Primer Probe Reagent|DUNS-153623137/PRD-06404:Panther Fusion SARS-CoV-2 Assay Controls|DUNS-153623137/PRD-06419:Aptima SARS-CoV-2 Assay Kit|DUNS-153623137/PRD-06420:Aptima SARS-CoV-2 Controls Kit|DUNS-153623137/PRD-06815:Aptima SARS-CoV-2/flu Assay Kit|DUNS-153623137/PRD-06816:Aptima SARS-CoV-2/flu Controls Kit|GLN-5060887160001/BCUBE 2.0:Bcube 2.0|GLN-5060887160001/BKTH-SCV2.02-32:Bkit Virus Finder COVID-19|GLN-5060887160001/HYCT16.01:16wells Cartridges|GLN-5060887160001/HYCT36.01:36-wells Cartridges|GLN-0816270020002/20026121:Idt For Illumina Nextera Dna Unique Dual Indexes Set A (96 Indexes, 96 Samples)|GLN-0816270020002/20026930:Idt For Illumina Nextera Dna Unique Dual Indexes Set B (96 Indexes, 96 Samples)|GLN-0816270020002/20026933:Idt For Illumina Nextera Dna Unique Dual Indexes Set D (96 Indexes, 96 Samples)|GLN-0816270020002/20026934:Idt For Illumina Nextera Dna Unique Dual Indexes Set C (96 Indexes, 96 Samples)|GLN-0816270020002/20043401:Illumina COVIDseq Positive Control Ht|GLN-0816270020002/20043434:Illumina COVIDseq Test Box 2 - 3072 Samples|GLN-0816270020002/20043436:Illumina COVIDseq Test Box 4 - 3072 Samples|GLN-0816270020002/20043439:Illumina COVIDseq Test Box 7 - 3072 Samples|GLN-0816270020002/20043641:Illumina Dragen COVIDseq Test Pipeline|GLN-0816270020002/20043645:Illumina COVIDseq Test Box 1 - 3072 Samples|GLN-0816270020002/20043646:Illumina COVIDseq Test Box 3 - 3072 Samples|GLN-0816270020002/20043647:Illumina COVIDseq Test Box 6 - 3072 Samples|GLN-0816270020002/20043648:Illumina COVIDseq Test Box 5 - 3072 Samples|DUNS-004006628/COV2-C:Smart Detect SARS-CoV-2 Rrt-PCR Kit|DUNS-243942278/B25-CSER1001:Lumivi Diagnostics SARS-CoV-2 IgG Rapid Test Kit|GLN-0850021628000/COV219:Kantaro Quantitative SARS-CoV-2 IgG Antibody Kit|GLN-0810055970001/00810055970056:Lucira Checkit COVID-19 Test Kit|GLN-0840487100004/50-10047:Aries SARS-CoV-2 Assay|DUNS-255371916/I054C0463:Nxtag Cov Extended Panel|CRN-842762684/GCRNA-ADVISO-96R:Genecount Clinical Advanced Rna Isolation Kit|CRN-842762684/GCRNA-AUTOISO-96R:Genecount Clinical Auto Rna Isolation Kit|CRN-842762684/GCRNA-COVID-96R:Genecount COVID-19 Rt-qPCR Assay Kit|CRN-842762684/QC-E32-EQP:Genecount E-32 Auto Purification Instrument|CRN-842762684/QC-Q16FL-PAC:Genecount Q-16, Flxl, Real Time QPCR Equip Set|CRN-842762684/QC-Q16FLXL-PAC:Genecount Q-16, Flxl, Real Time QPCR Equip Set|CRN-842762684/QC-Q96-EQP:Genecount Q-96, Flxl, Real Time QPCR Equip Set|GLN-4065384000004/243001N-10:Nadal COVID-19 IgG/IgM Test (pack Of 10)|GLN-4065384000004/243001N-10CA:Nadal COVID-19 IgG/IgM Test (pack Of 10, Canada)|GLN-4065384000004/243001N-100CA:Nadal COVID-19 IgG/IgM Test (pack Of 100, Canada)|GLN-4065384000004/243001N-20CA:Nadal COVID-19 IgG/IgM Test (pack Of 20, Canada)|GLN-4065384000004/243001N-50CA:Nadal COVID-19 IgG/IgM Test (pack Of 50, Canada)|CRN-330215000039151/XC25073:SARS-CoV-2 Virus Detection Diagnostic Kit (rt-qPCR Method)|LEI-549300ZZX9WCBZNYL849/619 9919:Vitros Immunodiagnostic Products Anti-SARS-CoV-2 IgG Reagent Pack|LEI-549300ZZX9WCBZNYL849/619 9920:Vitros Immunodiagnostic Products Anti-SARS-CoV-2 IgG Calibrator|LEI-549300ZZX9WCBZNYL849/619 9921:Vitros Immunodiagnostic Products Anti-SARS-CoV-2 IgG Controls|LEI-549300ZZX9WCBZNYL849/619 9943:Vitros Immunodiagnostic Products SARS-CoV-2 Antigen Controls|LEI-549300ZZX9WCBZNYL849/619 9944:Vitros Immunodiagnostic Products SARS-CoV-2 Antigen Extraction Buffer|LEI-549300ZZX9WCBZNYL849/619 9949:Vitros Immunodiagnostic Products SARS-CoV-2 Antigen Reagent Pack|LEI-549300ZZX9WCBZNYL849/619 9950:Vitros Immunodiagnostic Products SARS-CoV-2 Antigen Calibrator|GLN-0758750000008/619 9922:Vitros Immunodiagnostic Products Anti-SARS-CoV-2 Total Reagent Pack|GLN-0758750000008/619 9923:Vitros Immunodiagnostic Products Anti-SARS-CoV-2 Total Calibrator|GLN-0758750000008/619 9924:Vitros Immunodiagnostic Products Anti-SARS-CoV-2 Total Controls|GLN-0885502000006/IFMR-45:Genefinder COVID-19 Plus Realamp Kit|GLN-8800047500011/ATPI04:Pcl Immunofluorescence Analyzer Pclok Ez|GLN-8800047500011/COV05:Pcl COVID19 AG Rapid Fia|GLN-4053228000006/691223:Qiastat-dx Respiratory SARS-co V-2 Panel|GLN-4053228000006/9002813:Qiastat-dx Operational Module|GLN-4053228000006/9002814:Qiastat-dx Analytical Module|GLN-4053228000006/9002824:Qiastat-dx Analyzer 1.0|GLN-0014613000005/20374:Sofia SARS Antigen Fia|GLN-0014613000005/20377:Sofia 2 Flu + SARS Antigen Fia|GLN-0014613000005/20378:Sofia SARS Antigen Fia|GLN-0014613000005/20380:Sofia 2 Flu + SARS Antigen Fia|GLN-0014613000005/20391:Sofia 2 Flu + SARS Antigen Control Set|GLN-0014613000005/20398:Quickvue At-home Otc COVID-19 Test|GLN-0014613000005/20399:Quickvue At-home Otc COVID-19 Test|GLN-0014613000005/20402:Quickvue At-home Otc COVID-19 Test|GLN-0812589020009/SARS-COV-2-PCR-CAN:Perkinelmer New Coronavirus Nucleic Acid Detection Kit|CRN-743768921/F000003:Triplelock SARS-CoV-2 Tests|CRN-743768921/F000004:Triplelock SARS-CoV-2 Tests|CRN-743768921/F000010:Triplelock SARS-CoV-2 Tests|CRN-743768921/F000011:Triplelock SARS-CoV-2 Tests|CRN-743768921/F000012:Triplelock SARS-CoV-2 Tests|CRN-743768921/W000003:Triplelock SARS-CoV-2 Tests|CRN-743768921/W000007:Triplelock SARS-CoV-2 Tests|GLN-4038377000008/09203079190:Elecsys Anti-SARS-CoV-2|GLN-4038377000008/09203095190:Elecsys Anti-SARS-CoV-2|GLN-4038377000008/09216928190:Preci Control Anti-SARS-CoV-2|GLN-4038377000008/09289267190:Elecsys Anti-SARS-CoV-2 S|GLN-4038377000008/09289275190:Elecsys Anti-SARS-CoV-2 S|GLN-4038377000008/09289291190:Calset Anti-SARS-CoV-2 S|GLN-4038377000008/09289313190:Precicontrol Anti-SARS-CoV-2 S|GLN-0875197000009/09175431190:Cobas SARS-CoV-2 Test|GLN-0875197000009/09175440190:Cobas SARS-CoV-2 Control Kit|GLN-0875197000009/09211101190:Cobas SARS-CoV-2 &amp; Influenza A/b|GLN-0875197000009/09211128190:Cobas Liat SARS-CoV-2 &amp; Influenza A/b Quality Control Kit|GLN-0875197000009/09233474190:Cobas SARS-CoV-2 &amp; Influenza A/b|GLN-0875197000009/09233482190:Cobas SARS-CoV-2 &amp; Influenza A/b Control Kit|GLN-0875197000009/09255427001:Sw Cobas-CoV-2|GLN-0875197000009/09255478001:Sw Cobas-CoV-2|GLN-0875197000009/09259848001:Sw Cobas-CoV-2|GLN-0875197000009/09259856001:Sw Cobas-CoV-2|GLN-0875197000009/09260935001:Cobas Liat SARS-CoV-2 &amp; Influenza A/b Script Software Version 1.0|GLN-0875197000009/09343733190:Cobas SARS-CoV-2|GLN-0875197000009/09463526001:Cobas Liat SARS CoV-2 &amp; Influenza A/b Assay Script V1.1|GLN-0875197000009/09826009001:Sw Cobas Scov2-flua/b Asap V 12.1.0|GLN-0875197000009/09826017001:Sw Cobas Scov2-flua/b Asap V 11.1.0|GLN-0875197000009/09826041001:Sw Cobas Scov2-flua/b Asap V 10.1.0|GLN-0875197000009/09947060001:Sw Cobas SARS-CoV-2 Asap V11.3.0|GLN-0875197000009/09947078001:Sw Cobas SARS-CoV-2 Asap V10.3.0|DUNS-421167832/S3102E:COVID 19 Nucleic Acid Detection Kit (PCR-fluorescence Probing)|GLN-8800111700019/09COV31D:Standard Q COVID-19 AG Test|GLN-8800111700019/09COV33D:Standard Q COVID-19 AG Test With Control|GLN-8800111700019/9901-C-NCOV-01G:SARS-CoV-2 Antigen Control|GLN-8800111700019/9901-NCOV-01G:SARS-CoV-2 Rapid Antigen Test|GLN-8800111700019/9901-NCOV-03G:SARS-CoV-2 Rapid Antigen Test Nasal With Control|GLN-8800111700019/9901-NCOV-04G:SARS-CoV-2 Rapid Antigen Test Nasal|GLN-8800111700019/C-NCOV-01G:Standard COVID-19 AG Control|GLN-8800111700019/Q-NCOV-01G:Standard Q COVID-19 AG Test|GLN-8800069800014/SS-9030:U-top COVID-19 Detection Kit|GLN-8800069800014/SS-9030COE:U-top COVID-19 Detection Kit|GLN-8800069800014/SS-9030COM:U-top COVID-19 Detection Kit|GLN-8800069800014/SS-9030CON:U-top COVID-19 Detection Kit|GLN-8800069800014/SS-9030COP:U-top COVID-19 Detection Kit|GLN-8800069800014/SS-9030COS:U-top COVID-19 Detection Kit|GLN-8809240100011/RP10243X:Allplex 2019-NCoV Assay|CRN-310115000888557/RR-0487-02-50:Novel Coronavirus (SARS-CoV-2) Real-time Multiplex Rt-PCR Kit|CRN-310115000888557/RR-0487-02-200:Novel Coronavirus (SARS-CoV-2) Real-time Multiplex Rt-PCR Kit|GLN-0842768000003/11206710:Advia Centaur SARS-CoV-2 Total (cov2t)|GLN-0842768000003/11206711:Atellica Im SARS-CoV-2 Total (cov2t)|GLN-0842768000003/11206712:Atellica Im SARS-CoV-2-total Quality Control (cov2t Qc)|GLN-0842768000003/11206713:Advia Centaur SARS CoV-2 Total Quality Control (cov2t Qc)|GLN-0842768000003/11206922:Advia Centaur SARS-CoV-2 Total (cov2t)|GLN-0842768000003/11206923:Atellica Im SARS-CoV-2 Total (cov2t)|GLN-0842768000003/K7414:Dimension Vista SARS-CoV-2 Total Antibody (cov2t)|GLN-0842768000003/KC813:Dimension Vista/dimension Exl SARS-CoV-2 Total Antibody Calibrator (cov2t Cal/cv2t Cal)|GLN-0842768000003/KC815:Dimension Vista/dimension Exl SARS-CoV-2 Total Antibody Quality Control (cov2t/cv2t Pos/neg)|GLN-0842768000003/RF812:Dimension Exl SARS-CoV-2 Total Antibody (cv2t) Assay|GLN-8809517360018/SQD52-K020:Diaplexq Novel Coronavirus (2019-NCoV) Detection Kit|GLN-8809517360018/SQD52-K100:Diaplexq Novel Coronavirus (2019-NCoV) Detection Kit|DUNS-243605917/ASM-0174:Spartan COVID-19 System Sample Preparation Kit|DUNS-243605917/ASM-00144:Spartan COVID-19 System Test Cartridge|DUNS-243605917/ASM-00145:Spartan COVID-19 System Computer|DUNS-243605917/ASM-00146:Spartan COVID-19 System Cube|DUNS-243605917/ASM-00173:Spartan COVID-19 System Specimen Tube|DUNS-243605917/OTS-00233:Spartan COVID-19 System Barcode Scanner|DUNS-243605917/OTS-00307:Spartan COVID-19 System Usb Hub|GLN-0850000184008/A47814:Taqpath COVID-19 Combo Kit|GLN-0850000184008/A47817:Taqpath COVID-19 Rt-PCR Kit|GLN-0850000184008/A48002:Taqpath COVID-19 Control Dilution Buffer|GLN-0850000184008/A48003:Taqpath COVID-19 Control Kit|GLN-0850000184008/A49869:Taqpath COVID-19 High Throughput Combo Kit|GLN-0850000184008/COVID-19 SOFTWARE V1.3:Applied Biosystems COVID-19 Interpretive Software|GLN-0850000184008/COVID-19 SOFTWARE V2.3:Applied Biosystems COVID-19 Interpretive Software|CRN-350200200037950/09167:Rapid SARS-CoV-2 Antigen Test Card|CRN-350200200037950/061254:Rapid SARS-CoV-2 Antigen Test Card|CRN-350200200037950/1N40C5:Rapid SARS-CoV-2 Antigen Test Card|CRN-350200200037950/1N40T0:Rapid SARS-CoV-2 Antigen Test Card</t>
+  </si>
+  <si>
+    <t>Test information|Test type</t>
+  </si>
+  <si>
+    <t>GLN-8800075500014/M22MD100M|GLN-0811877010005/190-080|GLN-0811877010005/191-000|GLN-0813337010006/06R8601|GLN-0813337010006/06R8610|GLN-0813337010006/06R8620|GLN-0813337010006/06R8630|GLN-0813337010006/06R9001|GLN-0813337010006/06R9010|GLN-0813337010006/06R9020|GLN-0813337010006/06R9030|GLN-0884999000001/09N77-001|GLN-0884999000001/09N77-010|GLN-0884999000001/09N77-080|GLN-0884999000001/09N77-085|GLN-0884999000001/09N77-090|GLN-0884999000001/09N77-095|GLN-0884999000001/09N78-080|GLN-0884999000001/09N78-090|GLN-0884999000001/09N79-080|GLN-0884999000001/09N79-090|GLN-4051892000001/41FK10|GLN-4051892000001/41FK11|LEI-549300883RE115J3LD19/A03-51-322|CRN-2354710/COV-W23M|GLN-0382900000008/256082|GLN-0382900000008/256089|GLN-0382900000008/445003-01|DUNS-962942756/MFG030018|GLN-0851458005006/423744|GLN-0851458005006/423748|GLN-0815381020000/423738|GLN-0860004739708/1000003|GLN-0860004739708/1000012|GLN-0860004739708/1000013|GLN-0860004739708/1000018|GLN-0860004739708/3000011|GLN-0860004739708/3000150|GLN-0860004739708/3000536|GLN-0860004739708/3000555|GLN-0860004739708/3000562|GLN-0860004739708/3000563|GLN-0860004739708/3000564|GLN-0860004739708/3000567|GLN-3015730200108/423720|GLN-3610520000007/72710|GLN-3610520000007/12013798|DUNS-251005005/COV-13C25|DUNS-956711444/XPCOV2/FLU/RSV-10|DUNS-956711444/XPRSARS-COV2-10|GLN-0810040820007/C0200|GLN-0810040820007/C0201|GLN-0810040820007/C1021-01|GLN-0810040820007/C1021-03|GLN-0810040820007/C1021-10|GLN-0810040820007/C1021-100|GLN-0810040820007/C2113|GLN-0810040820007/CUE HEALTH APP|CRN-103082/CAN-IGG-19|CRN-103082/CAN-IGT-19|GLN-0014613000005/M120|GLN-0014613000005/M124|GLN-0014613000005/M313|DUNS-033429783/311460|DUNS-033429783/311461|GLN-0816101020003/MOL4150|GLN-0816101020003/MOL4160|GLN-0893230002001/KT-1032|GLN-4049016000006/EI 2606-9601 G|GLN-4049016000006/MP 2606-0100|GLN-4049016000006/MP 2606-0125|GLN-4049016000006/MP 2606-0200|GLN-4049016000006/MP 2606-0225|GLN-4049016000006/MP 2606-0425|GLN-4049016000006/MP 2606-1000|GLN-5453003370000/11416302 (FTD-114-96)|DUNS-153623137/PRD-03546|DUNS-153623137/PRD-04303|DUNS-153623137/PRD-04304|DUNS-153623137/PRD-04331|DUNS-153623137/PRD-04332|DUNS-153623137/PRD-04334|DUNS-153623137/PRD-04335|DUNS-153623137/PRD-06391|DUNS-153623137/PRD-06404|DUNS-153623137/PRD-06419|DUNS-153623137/PRD-06420|DUNS-153623137/PRD-06815|DUNS-153623137/PRD-06816|GLN-5060887160001/BCUBE 2.0|GLN-5060887160001/BKTH-SCV2.02-32|GLN-5060887160001/HYCT16.01|GLN-5060887160001/HYCT36.01|GLN-0816270020002/20026121|GLN-0816270020002/20026930|GLN-0816270020002/20026933|GLN-0816270020002/20026934|GLN-0816270020002/20043401|GLN-0816270020002/20043434|GLN-0816270020002/20043436|GLN-0816270020002/20043439|GLN-0816270020002/20043641|GLN-0816270020002/20043645|GLN-0816270020002/20043646|GLN-0816270020002/20043647|GLN-0816270020002/20043648|DUNS-004006628/COV2-C|DUNS-243942278/B25-CSER1001|GLN-0850021628000/COV219|GLN-0810055970001/00810055970056|GLN-0840487100004/50-10047|DUNS-255371916/I054C0463|CRN-842762684/GCRNA-ADVISO-96R|CRN-842762684/GCRNA-AUTOISO-96R|CRN-842762684/GCRNA-COVID-96R|CRN-842762684/QC-E32-EQP|CRN-842762684/QC-Q16FL-PAC|CRN-842762684/QC-Q16FLXL-PAC|CRN-842762684/QC-Q96-EQP|GLN-4065384000004/243001N-10|GLN-4065384000004/243001N-10CA|GLN-4065384000004/243001N-100CA|GLN-4065384000004/243001N-20CA|GLN-4065384000004/243001N-50CA|CRN-330215000039151/XC25073|LEI-549300ZZX9WCBZNYL849/619 9919|LEI-549300ZZX9WCBZNYL849/619 9920|LEI-549300ZZX9WCBZNYL849/619 9921|LEI-549300ZZX9WCBZNYL849/619 9943|LEI-549300ZZX9WCBZNYL849/619 9944|LEI-549300ZZX9WCBZNYL849/619 9949|LEI-549300ZZX9WCBZNYL849/619 9950|GLN-0758750000008/619 9922|GLN-0758750000008/619 9923|GLN-0758750000008/619 9924|GLN-0885502000006/IFMR-45|GLN-8800047500011/ATPI04|GLN-8800047500011/COV05|GLN-4053228000006/691223|GLN-4053228000006/9002813|GLN-4053228000006/9002814|GLN-4053228000006/9002824|GLN-0014613000005/20374|GLN-0014613000005/20377|GLN-0014613000005/20378|GLN-0014613000005/20380|GLN-0014613000005/20391|GLN-0014613000005/20398|GLN-0014613000005/20399|GLN-0014613000005/20402|GLN-0812589020009/SARS-COV-2-PCR-CAN|CRN-743768921/F000003|CRN-743768921/F000004|CRN-743768921/F000010|CRN-743768921/F000011|CRN-743768921/F000012|CRN-743768921/W000003|CRN-743768921/W000007|GLN-4038377000008/09203079190|GLN-4038377000008/09203095190|GLN-4038377000008/09216928190|GLN-4038377000008/09289267190|GLN-4038377000008/09289275190|GLN-4038377000008/09289291190|GLN-4038377000008/09289313190|GLN-0875197000009/09175431190|GLN-0875197000009/09175440190|GLN-0875197000009/09211101190|GLN-0875197000009/09211128190|GLN-0875197000009/09233474190|GLN-0875197000009/09233482190|GLN-0875197000009/09255427001|GLN-0875197000009/09255478001|GLN-0875197000009/09259848001|GLN-0875197000009/09259856001|GLN-0875197000009/09260935001|GLN-0875197000009/09343733190|GLN-0875197000009/09463526001|GLN-0875197000009/09826009001|GLN-0875197000009/09826017001|GLN-0875197000009/09826041001|GLN-0875197000009/09947060001|GLN-0875197000009/09947078001|DUNS-421167832/S3102E|GLN-8800111700019/09COV31D|GLN-8800111700019/09COV33D|GLN-8800111700019/9901-C-NCOV-01G|GLN-8800111700019/9901-NCOV-01G|GLN-8800111700019/9901-NCOV-03G|GLN-8800111700019/9901-NCOV-04G|GLN-8800111700019/C-NCOV-01G|GLN-8800111700019/Q-NCOV-01G|GLN-8800069800014/SS-9030|GLN-8800069800014/SS-9030COE|GLN-8800069800014/SS-9030COM|GLN-8800069800014/SS-9030CON|GLN-8800069800014/SS-9030COP|GLN-8800069800014/SS-9030COS|GLN-8809240100011/RP10243X|CRN-310115000888557/RR-0487-02-50|CRN-310115000888557/RR-0487-02-200|GLN-0842768000003/11206710|GLN-0842768000003/11206711|GLN-0842768000003/11206712|GLN-0842768000003/11206713|GLN-0842768000003/11206922|GLN-0842768000003/11206923|GLN-0842768000003/K7414|GLN-0842768000003/KC813|GLN-0842768000003/KC815|GLN-0842768000003/RF812|GLN-8809517360018/SQD52-K020|GLN-8809517360018/SQD52-K100|DUNS-243605917/ASM-0174|DUNS-243605917/ASM-00144|DUNS-243605917/ASM-00145|DUNS-243605917/ASM-00146|DUNS-243605917/ASM-00173|DUNS-243605917/OTS-00233|DUNS-243605917/OTS-00307|GLN-0850000184008/A47814|GLN-0850000184008/A47817|GLN-0850000184008/A48002|GLN-0850000184008/A48003|GLN-0850000184008/A49869|GLN-0850000184008/COVID-19 SOFTWARE V1.3|GLN-0850000184008/COVID-19 SOFTWARE V2.3|CRN-350200200037950/09167|CRN-350200200037950/061254|CRN-350200200037950/1N40C5|CRN-350200200037950/1N40T0</t>
+  </si>
+  <si>
+    <t>Carte de test d'antigène COVID-19</t>
+  </si>
+  <si>
+    <t>Un formulaire à utiliser pour les informations d'identification vérifiables du test d'antigène COVID-19 pour l'interopérabilité de base</t>
+  </si>
+  <si>
+    <t>Personnel/Opérationnel|ID de certificat de test lié</t>
+  </si>
+  <si>
+    <t>Identifiant unique du certificat de test associé</t>
+  </si>
+  <si>
+    <t>Informations sur le test|Maladie ou agent ciblé|Classification de la maladie</t>
+  </si>
+  <si>
+    <t>Maladie ou agent dont le test permet la détection.</t>
+  </si>
+  <si>
+    <t>Description du type de test effectué, par ex. TAAN ou test rapide d'antigène.</t>
+  </si>
+  <si>
+    <t>Informations sur le test|Nom commercial du test</t>
+  </si>
+  <si>
+    <t>Nom commercial ou de marque du test.</t>
+  </si>
+  <si>
+    <t>Informations sur le test|Fabricant de test</t>
+  </si>
+  <si>
+    <t>Fabricant légal du test.</t>
+  </si>
+  <si>
+    <t>Informations sur le test|Date et heure de la collecte de l'échantillon de test</t>
+  </si>
+  <si>
+    <t>Date et heure de prélèvement de l'échantillon.</t>
+  </si>
+  <si>
+    <t>Informations sur le test|Date et heure de la production du résultat du test</t>
+  </si>
+  <si>
+    <t>Date et heure de production du résultat du test.</t>
+  </si>
+  <si>
+    <t>Informations sur le test|Résultat du test</t>
+  </si>
+  <si>
+    <t>Par exemple, négatif, positif, non concluant ou nul.</t>
+  </si>
+  <si>
+    <t>Informations sur le test|Centre ou installation de test</t>
+  </si>
+  <si>
+    <t>Nom/code du centre de test, de l'établissement ou d'une autorité sanitaire responsable de l'événement de test.</t>
+  </si>
+  <si>
+    <t>Informations sur le test|Province ou territoire où le test a été effectué</t>
+  </si>
+  <si>
+    <t>La province ou le territoire où la personne a été testée</t>
+  </si>
+  <si>
+    <t>Informations sur le test|Pays où le test a été effectué</t>
+  </si>
+  <si>
+    <t>Le pays dans lequel l'individu a été testé.</t>
+  </si>
+  <si>
+    <t>Informations sur le test|Type de test</t>
+  </si>
+  <si>
+    <t>GLN-8800075500014:1drop Inc. (Corée du Sud)|GLN-0811877010005:Abbott Diagnostics Scarborough, Inc. (États-Unis)|GLN-0813337010006:Abbott Laboratories Diagnostics Division (États-Unis)|GLN-0884999000001:Abbott Molecular Inc. (États-Unis)|GLN-4051892000001:Abbott Rapid Diagnostics Jena Gmbh (Allemagne)|LEI-549300883RE115J3LD19:Artron Laboratories Inc. (Canada)|CRN-2354710:Assure Tech. (Hangzhou) Co. Ltd. (Chine)|GLN-0382900000008:Becton Dickinson And Company (Bd) (États-Unis)|DUNS-962942756:Bgi Americas Corp (États-Unis)|GLN-0851458005006:Biofire Defense (États-Unis)|GLN-0815381020000:Biofire Diagnostics, Llc. (États-Unis)|GLN-0860004739708:Biomeme Inc (États-Unis)|GLN-3015730200108:Biomerieux Sa (France)|GLN-3610520000007:Bio-Rad (France)|DUNS-251005005:Btnx Inc. (Canada)|DUNS-956711444:Cepheid (États-Unis)|GLN-0810040820007:Cue Health Inc. (États-Unis)|CRN-103082:Diagnostics Biochem Canada Inc. (Canada)|GLN-0014613000005:Diagnostic Hybrids, Inc. - Négociant également en tant que Quidel Corporation (États-Unis)|DUNS-033429783:Diasorin Inc. (États-Unis)|GLN-0816101020003:Diasorin Molecular Llc (États-Unis)|GLN-0893230002001:Epitope Diagnostics, Inc. (États-Unis)|GLN-4049016000006:Euroimmun Medizinische Labordiagnostika Ag (Allemagne)|GLN-5453003370000:Fast Track Diagnostics Luxembourg S.A.R.L. (Luxembourg)|DUNS-153623137:Hologic, Inc. (États-Unis)|GLN-5060887160001:Hyris Ltd (Grande-Bretagne)|GLN-0816270020002:Illumina, Inc. (États-Unis)|DUNS-004006628:Inbios International Inc. (États-Unis)|DUNS-243942278:International Point Of Care, Inc. (Canada)|GLN-0850021628000:Kantaro Biosciences, Llc (États-Unis)|GLN-0810055970001:Lucira Health, Inc. (États-Unis)|GLN-0840487100004:Luminex Corporation (États-Unis)|DUNS-255371916:Luminex Molecular Diagnostics, Inc. (Canada)|CRN-842762684:Luminultra Technologies Ltd. (Canada)|GLN-4065384000004:Nal Von Minden Gmbh (Allemagne)|CRN-330215000039151:Ningbo Health Gene Technologies Co., Ltd (Chine)|LEI-549300ZZX9WCBZNYL849:Ortho-Clinical Diagnostics (Grande-Bretagne)|GLN-0758750000008:Ortho-Clinical Diagnostics Inc. (États-Unis)|GLN-0885502000006:Osang Healthcare Co., Ltd. (Corée du Sud)|GLN-8800047500011:Pcl Inc. (Corée du Sud)|GLN-4053228000006:Qiagen Gmbh (Allemagne)|GLN-0014613000005:Quidel Corporation (États-Unis)|GLN-0812589020009:Perkinelmer, Inc. (États-Unis)|CRN-743768921:Precision Biomonitoring Inc. (Canada)|GLN-4038377000008:Roche Diagnostics Gmbh (Allemagne)|GLN-0875197000009:Roche Molecular Systems, Inc (États-Unis)|DUNS-421167832:Sansure Biotech Inc. (Chine)|GLN-8800111700019:Sd Biosensor, Inc. (Corée du Sud)|GLN-8800069800014:Seasun Biomaterials Inc. (Corée du Sud)|GLN-8809240100011:Seegene Inc. (Corée du Sud)|CRN-310115000888557:Shanghai Zj Bio-Tech Co., Ltd (Chine)|GLN-0842768000003:Siemens Healthcare Diagnostics Inc. (États-Unis)|GLN-8809517360018:Solgent Co., Ltd. (Corée du Sud)|DUNS-243605917:Spartan Bioscience Inc. (Canada)|GLN-0850000184008:Thermo Fisher Scientific (États-Unis)|CRN-350200200037950:Xiamen Boson Biotech Co., Ltd. (Chine)</t>
+  </si>
+  <si>
+    <t>260415000:Non-détecté|260373001:Détecté</t>
+  </si>
+  <si>
+    <t>LP6464-4:Sonde avec amplification de la cible|LP217198-3:IA.rapide</t>
+  </si>
+  <si>
+    <t>GLN, DUNS, LEI or CRN (+ device identifiers)</t>
+  </si>
+  <si>
+    <t>GLN, DUNS, LEI or CRN</t>
+  </si>
+  <si>
+    <t>GLN = Global Location Number</t>
+  </si>
+  <si>
+    <t>DUNS = Data Universal Numbering System [Dun &amp; Bradstreet]</t>
+  </si>
+  <si>
+    <t>LEI = Legal Entity Identifier</t>
+  </si>
+  <si>
+    <t>CRN = Company Registration Number</t>
+  </si>
+  <si>
+    <r>
+      <t>An </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Entry Codes Overlay</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t> is a core linked object that defines coded value sets. A value set specifies a set of codes drawn from one or more code systems, intended for use in a particular context. Value sets link between code system definitions and their use in coded elements.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Vaccination Credential
+COVID-19 Antigen Test Credential
+</t>
+  </si>
+  <si>
+    <t>LEI-549300EI6OKH5K5Q2G38:MODERNA, INC.|LEI-765LHXWGK1KXCLTFYQ30:PFIZER INC.|LEI-PY6ZZQWO2IZFZC3IOL08:ASTRAZENECA PLC|LEI-549300YLGMXJV7RFQN72:JANSSEN-CILAG B.V.</t>
+  </si>
+  <si>
+    <t>LEI</t>
+  </si>
+  <si>
+    <t>LEI-549300EI6OKH5K5Q2G38|LEI-765LHXWGK1KXCLTFYQ30|LEI-PY6ZZQWO2IZFZC3IOL08|LEI-549300YLGMXJV7RFQN72</t>
   </si>
 </sst>
 </file>
@@ -1297,7 +1559,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1382,8 +1644,20 @@
         <bgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="69">
+  <borders count="70">
     <border>
       <left/>
       <right/>
@@ -2241,6 +2515,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="3" tint="0.59999389629810485"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3" tint="0.59999389629810485"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
@@ -2253,7 +2540,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="164">
+  <cellXfs count="182">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -2627,6 +2914,48 @@
     <xf numFmtId="0" fontId="31" fillId="14" borderId="48" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="50" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="15" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="16" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="15" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="16" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="15" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="16" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="58" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="59" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="60" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2693,6 +3022,12 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -4608,7 +4943,7 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="B1:D979"/>
+  <dimension ref="B1:D984"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="92" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -4627,50 +4962,50 @@
         <v>141</v>
       </c>
       <c r="C1" s="130" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D1" s="85"/>
     </row>
     <row r="2" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="160"/>
-      <c r="C2" s="160"/>
-      <c r="D2" s="160"/>
+      <c r="B2" s="176"/>
+      <c r="C2" s="176"/>
+      <c r="D2" s="176"/>
     </row>
     <row r="3" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="161"/>
-      <c r="C3" s="161"/>
-      <c r="D3" s="161"/>
+      <c r="B3" s="177"/>
+      <c r="C3" s="177"/>
+      <c r="D3" s="177"/>
     </row>
     <row r="4" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="161"/>
-      <c r="C4" s="161"/>
-      <c r="D4" s="161"/>
+      <c r="B4" s="177"/>
+      <c r="C4" s="177"/>
+      <c r="D4" s="177"/>
     </row>
     <row r="5" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="162"/>
-      <c r="C5" s="162"/>
-      <c r="D5" s="162"/>
+      <c r="B5" s="178"/>
+      <c r="C5" s="178"/>
+      <c r="D5" s="178"/>
     </row>
     <row r="6" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B6" s="163"/>
-      <c r="C6" s="163"/>
-      <c r="D6" s="163"/>
+      <c r="B6" s="179"/>
+      <c r="C6" s="179"/>
+      <c r="D6" s="179"/>
     </row>
     <row r="7" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="95" t="s">
         <v>140</v>
       </c>
-      <c r="C7" s="153" t="s">
+      <c r="C7" s="169" t="s">
         <v>155</v>
       </c>
-      <c r="D7" s="154"/>
+      <c r="D7" s="170"/>
     </row>
     <row r="8" spans="2:4" ht="43" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="96" t="s">
         <v>154</v>
       </c>
       <c r="C8" s="97" t="s">
-        <v>196</v>
+        <v>304</v>
       </c>
       <c r="D8" s="98"/>
     </row>
@@ -4685,19 +5020,19 @@
       <c r="B10" s="92" t="s">
         <v>139</v>
       </c>
-      <c r="C10" s="155">
-        <v>42973</v>
-      </c>
-      <c r="D10" s="156"/>
+      <c r="C10" s="171">
+        <v>42986</v>
+      </c>
+      <c r="D10" s="172"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B11" s="91" t="s">
         <v>138</v>
       </c>
-      <c r="C11" s="136" t="s">
+      <c r="C11" s="152" t="s">
         <v>153</v>
       </c>
-      <c r="D11" s="137"/>
+      <c r="D11" s="153"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12" s="90"/>
@@ -4710,11 +5045,11 @@
       <c r="D13" s="89"/>
     </row>
     <row r="14" spans="2:4" ht="128.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B14" s="138" t="s">
+      <c r="B14" s="154" t="s">
         <v>160</v>
       </c>
-      <c r="C14" s="139"/>
-      <c r="D14" s="140"/>
+      <c r="C14" s="155"/>
+      <c r="D14" s="156"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B15" s="85"/>
@@ -4733,7 +5068,7 @@
       </c>
     </row>
     <row r="17" spans="2:4" ht="48" x14ac:dyDescent="0.15">
-      <c r="B17" s="148" t="s">
+      <c r="B17" s="164" t="s">
         <v>134</v>
       </c>
       <c r="C17" s="106"/>
@@ -4742,28 +5077,28 @@
       </c>
     </row>
     <row r="18" spans="2:4" ht="16" x14ac:dyDescent="0.15">
-      <c r="B18" s="151"/>
+      <c r="B18" s="167"/>
       <c r="C18" s="108" t="s">
         <v>133</v>
       </c>
       <c r="D18" s="107"/>
     </row>
     <row r="19" spans="2:4" ht="16" x14ac:dyDescent="0.15">
-      <c r="B19" s="151"/>
+      <c r="B19" s="167"/>
       <c r="C19" s="109" t="s">
         <v>168</v>
       </c>
       <c r="D19" s="107"/>
     </row>
     <row r="20" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B20" s="152"/>
+      <c r="B20" s="168"/>
       <c r="C20" s="108" t="s">
         <v>169</v>
       </c>
       <c r="D20" s="107"/>
     </row>
     <row r="21" spans="2:4" ht="59" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="148" t="s">
+      <c r="B21" s="164" t="s">
         <v>143</v>
       </c>
       <c r="C21" s="110" t="s">
@@ -4774,7 +5109,7 @@
       </c>
     </row>
     <row r="22" spans="2:4" ht="42" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B22" s="149"/>
+      <c r="B22" s="165"/>
       <c r="C22" s="106" t="s">
         <v>7</v>
       </c>
@@ -4783,7 +5118,7 @@
       </c>
     </row>
     <row r="23" spans="2:4" ht="41" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B23" s="149"/>
+      <c r="B23" s="165"/>
       <c r="C23" s="106" t="s">
         <v>8</v>
       </c>
@@ -4792,12 +5127,12 @@
       </c>
     </row>
     <row r="24" spans="2:4" ht="88" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B24" s="150"/>
+      <c r="B24" s="166"/>
       <c r="C24" s="106" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="D24" s="107" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="53" customHeight="1" x14ac:dyDescent="0.15">
@@ -4811,350 +5146,360 @@
         <v>173</v>
       </c>
     </row>
-    <row r="26" spans="2:4" ht="37" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B26" s="99" t="s">
+    <row r="26" spans="2:4" s="133" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B26" s="134" t="s">
         <v>145</v>
       </c>
       <c r="C26" s="106" t="s">
         <v>14</v>
       </c>
       <c r="D26" s="107" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" ht="50" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B27" s="99" t="s">
+        <v>223</v>
+      </c>
+      <c r="C27" s="106" t="s">
+        <v>192</v>
+      </c>
+      <c r="D27" s="107" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" ht="39" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B28" s="162" t="s">
+        <v>142</v>
+      </c>
+      <c r="C28" s="106" t="s">
+        <v>146</v>
+      </c>
+      <c r="D28" s="107" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="27" spans="2:4" ht="39" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B27" s="146" t="s">
-        <v>142</v>
-      </c>
-      <c r="C27" s="106" t="s">
-        <v>146</v>
-      </c>
-      <c r="D27" s="107" t="s">
+    <row r="29" spans="2:4" ht="39" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B29" s="163"/>
+      <c r="C29" s="106" t="s">
+        <v>147</v>
+      </c>
+      <c r="D29" s="107" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="28" spans="2:4" ht="39" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B28" s="147"/>
-      <c r="C28" s="106" t="s">
-        <v>147</v>
-      </c>
-      <c r="D28" s="107" t="s">
+    <row r="30" spans="2:4" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B30" s="87" t="s">
+        <v>148</v>
+      </c>
+      <c r="C30" s="106" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="107" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="29" spans="2:4" ht="54" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B29" s="87" t="s">
-        <v>148</v>
-      </c>
-      <c r="C29" s="106" t="s">
-        <v>16</v>
-      </c>
-      <c r="D29" s="107" t="s">
+    <row r="31" spans="2:4" ht="69" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B31" s="87" t="s">
+        <v>149</v>
+      </c>
+      <c r="C31" s="106" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="107" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="30" spans="2:4" ht="69" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B30" s="87" t="s">
-        <v>149</v>
-      </c>
-      <c r="C30" s="106" t="s">
-        <v>17</v>
-      </c>
-      <c r="D30" s="107" t="s">
+    <row r="32" spans="2:4" ht="38" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B32" s="87" t="s">
+        <v>150</v>
+      </c>
+      <c r="C32" s="106" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="107" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="31" spans="2:4" ht="38" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B31" s="87" t="s">
-        <v>150</v>
-      </c>
-      <c r="C31" s="106" t="s">
-        <v>18</v>
-      </c>
-      <c r="D31" s="107" t="s">
+    <row r="33" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B33" s="162" t="s">
+        <v>132</v>
+      </c>
+      <c r="C33" s="111"/>
+      <c r="D33" s="107" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B34" s="167"/>
+      <c r="C34" s="106" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="112" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="32" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B32" s="146" t="s">
-        <v>132</v>
-      </c>
-      <c r="C32" s="111"/>
-      <c r="D32" s="107" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B33" s="151"/>
-      <c r="C33" s="106" t="s">
-        <v>45</v>
-      </c>
-      <c r="D33" s="112" t="s">
+    <row r="35" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B35" s="167"/>
+      <c r="C35" s="106" t="s">
+        <v>0</v>
+      </c>
+      <c r="D35" s="107" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B36" s="167"/>
+      <c r="C36" s="106" t="s">
+        <v>43</v>
+      </c>
+      <c r="D36" s="112" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="34" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B34" s="151"/>
-      <c r="C34" s="106" t="s">
-        <v>0</v>
-      </c>
-      <c r="D34" s="107" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B35" s="151"/>
-      <c r="C35" s="106" t="s">
-        <v>43</v>
-      </c>
-      <c r="D35" s="112" t="s">
+    <row r="37" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B37" s="167"/>
+      <c r="C37" s="106" t="s">
+        <v>44</v>
+      </c>
+      <c r="D37" s="112" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="36" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B36" s="151"/>
-      <c r="C36" s="106" t="s">
-        <v>44</v>
-      </c>
-      <c r="D36" s="112" t="s">
+    <row r="38" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B38" s="167"/>
+      <c r="C38" s="106" t="s">
+        <v>213</v>
+      </c>
+      <c r="D38" s="112" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B39" s="167"/>
+      <c r="C39" s="106" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="112" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="37" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B37" s="151"/>
-      <c r="C37" s="106" t="s">
-        <v>218</v>
-      </c>
-      <c r="D37" s="112" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B38" s="151"/>
-      <c r="C38" s="106" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" s="112" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" ht="46" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B39" s="152"/>
-      <c r="C39" s="106"/>
-      <c r="D39" s="107" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" ht="16" x14ac:dyDescent="0.15">
-      <c r="B40" s="87" t="s">
-        <v>129</v>
-      </c>
+    <row r="40" spans="2:4" ht="46" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B40" s="168"/>
       <c r="C40" s="106"/>
       <c r="D40" s="107" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" ht="16" x14ac:dyDescent="0.15">
+      <c r="B41" s="87" t="s">
+        <v>129</v>
+      </c>
+      <c r="C41" s="106"/>
+      <c r="D41" s="107" t="s">
         <v>128</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="113" t="s">
-        <v>184</v>
-      </c>
-      <c r="C41" s="114"/>
-      <c r="D41" s="107" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="42" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="113" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C42" s="114"/>
       <c r="D42" s="107" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="113" t="s">
+        <v>185</v>
+      </c>
+      <c r="C43" s="114"/>
+      <c r="D43" s="107" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="115" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="43" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="115" t="s">
+      <c r="C44" s="116"/>
+      <c r="D44" s="107" t="s">
         <v>188</v>
-      </c>
-      <c r="C43" s="116"/>
-      <c r="D43" s="107" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="86" t="s">
-        <v>127</v>
-      </c>
-      <c r="C44" s="117"/>
-      <c r="D44" s="107" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="45" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="86" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C45" s="117"/>
       <c r="D45" s="107" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="46" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="86" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C46" s="117"/>
       <c r="D46" s="107" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="47" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="86" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C47" s="117"/>
       <c r="D47" s="107" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4" s="121" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="132" t="s">
-        <v>214</v>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="86" t="s">
+        <v>121</v>
       </c>
       <c r="C48" s="117"/>
       <c r="D48" s="107" t="s">
-        <v>217</v>
+        <v>120</v>
       </c>
     </row>
     <row r="49" spans="2:4" s="121" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="132" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="C49" s="117"/>
       <c r="D49" s="107" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="103"/>
-      <c r="C50" s="103"/>
-      <c r="D50" s="103"/>
+        <v>212</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" s="121" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B50" s="132" t="s">
+        <v>210</v>
+      </c>
+      <c r="C50" s="117"/>
+      <c r="D50" s="107" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="51" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B51" s="157" t="s">
+      <c r="B51" s="103"/>
+      <c r="C51" s="103"/>
+      <c r="D51" s="103"/>
+    </row>
+    <row r="52" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B52" s="173" t="s">
         <v>119</v>
       </c>
-      <c r="C51" s="158"/>
-      <c r="D51" s="159"/>
-    </row>
-    <row r="52" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B52" s="143" t="s">
+      <c r="C52" s="174"/>
+      <c r="D52" s="175"/>
+    </row>
+    <row r="53" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B53" s="159" t="s">
         <v>151</v>
       </c>
-      <c r="C52" s="144"/>
-      <c r="D52" s="145"/>
-    </row>
-    <row r="53" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B53" s="100" t="s">
-        <v>152</v>
-      </c>
-      <c r="D53" s="102"/>
+      <c r="C53" s="160"/>
+      <c r="D53" s="161"/>
     </row>
     <row r="54" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B54" s="100" t="s">
-        <v>197</v>
+        <v>152</v>
       </c>
       <c r="D54" s="102"/>
     </row>
     <row r="55" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="100" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="D55" s="102"/>
     </row>
-    <row r="56" spans="2:4" s="121" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B56" s="120" t="s">
-        <v>157</v>
-      </c>
-      <c r="D56" s="122"/>
+    <row r="56" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B56" s="100" t="s">
+        <v>189</v>
+      </c>
+      <c r="D56" s="102"/>
     </row>
     <row r="57" spans="2:4" s="121" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="120" t="s">
-        <v>220</v>
+        <v>157</v>
       </c>
       <c r="D57" s="122"/>
     </row>
-    <row r="58" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B58" s="100" t="s">
-        <v>221</v>
-      </c>
-      <c r="D58" s="102"/>
-    </row>
-    <row r="59" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B59" s="133" t="s">
+    <row r="58" spans="2:4" s="121" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B58" s="120" t="s">
         <v>156</v>
       </c>
-      <c r="C59" s="134"/>
-      <c r="D59" s="135"/>
-    </row>
-    <row r="60" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B60" s="118"/>
-      <c r="C60" s="101"/>
-      <c r="D60" s="119"/>
-    </row>
-    <row r="61" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B61" s="118"/>
-      <c r="C61" s="101"/>
-      <c r="D61" s="119"/>
-    </row>
-    <row r="62" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B62" s="103"/>
-      <c r="C62" s="103"/>
-      <c r="D62" s="103"/>
-    </row>
-    <row r="63" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B63" s="141" t="s">
-        <v>198</v>
-      </c>
-      <c r="C63" s="141"/>
-      <c r="D63" s="141"/>
+      <c r="D58" s="122"/>
+    </row>
+    <row r="59" spans="2:4" s="146" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B59" s="145" t="s">
+        <v>215</v>
+      </c>
+      <c r="D59" s="147"/>
+    </row>
+    <row r="60" spans="2:4" s="146" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B60" s="145" t="s">
+        <v>216</v>
+      </c>
+      <c r="D60" s="147"/>
+    </row>
+    <row r="61" spans="2:4" s="146" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B61" s="145" t="s">
+        <v>299</v>
+      </c>
+      <c r="D61" s="147"/>
+    </row>
+    <row r="62" spans="2:4" s="146" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B62" s="145" t="s">
+        <v>300</v>
+      </c>
+      <c r="D62" s="147"/>
+    </row>
+    <row r="63" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B63" s="100" t="s">
+        <v>301</v>
+      </c>
+      <c r="D63" s="102"/>
     </row>
     <row r="64" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B64" s="142" t="s">
-        <v>199</v>
-      </c>
-      <c r="C64" s="142"/>
-      <c r="D64" s="142"/>
+      <c r="B64" s="149" t="s">
+        <v>302</v>
+      </c>
+      <c r="C64" s="150"/>
+      <c r="D64" s="151"/>
     </row>
     <row r="65" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B65" s="103"/>
-      <c r="C65" s="103"/>
-      <c r="D65" s="103"/>
+      <c r="B65" s="118"/>
+      <c r="C65" s="101"/>
+      <c r="D65" s="119"/>
     </row>
     <row r="66" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B66" s="85"/>
-      <c r="C66" s="85"/>
-      <c r="D66" s="85"/>
+      <c r="B66" s="118"/>
+      <c r="C66" s="101"/>
+      <c r="D66" s="119"/>
     </row>
     <row r="67" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B67" s="85"/>
-      <c r="C67" s="85"/>
-      <c r="D67" s="85"/>
-    </row>
-    <row r="68" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B68" s="85"/>
-      <c r="C68" s="85"/>
-      <c r="D68" s="85"/>
+      <c r="B67" s="103"/>
+      <c r="C67" s="103"/>
+      <c r="D67" s="103"/>
+    </row>
+    <row r="68" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B68" s="157" t="s">
+        <v>196</v>
+      </c>
+      <c r="C68" s="157"/>
+      <c r="D68" s="157"/>
     </row>
     <row r="69" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="85"/>
-      <c r="C69" s="85"/>
-      <c r="D69" s="85"/>
+      <c r="B69" s="158" t="s">
+        <v>197</v>
+      </c>
+      <c r="C69" s="158"/>
+      <c r="D69" s="158"/>
     </row>
     <row r="70" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B70" s="85"/>
-      <c r="C70" s="85"/>
-      <c r="D70" s="85"/>
+      <c r="B70" s="103"/>
+      <c r="C70" s="103"/>
+      <c r="D70" s="103"/>
     </row>
     <row r="71" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B71" s="85"/>
@@ -9701,80 +10046,105 @@
       <c r="C979" s="85"/>
       <c r="D979" s="85"/>
     </row>
+    <row r="980" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B980" s="85"/>
+      <c r="C980" s="85"/>
+      <c r="D980" s="85"/>
+    </row>
+    <row r="981" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B981" s="85"/>
+      <c r="C981" s="85"/>
+      <c r="D981" s="85"/>
+    </row>
+    <row r="982" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B982" s="85"/>
+      <c r="C982" s="85"/>
+      <c r="D982" s="85"/>
+    </row>
+    <row r="983" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B983" s="85"/>
+      <c r="C983" s="85"/>
+      <c r="D983" s="85"/>
+    </row>
+    <row r="984" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B984" s="85"/>
+      <c r="C984" s="85"/>
+      <c r="D984" s="85"/>
+    </row>
   </sheetData>
   <mergeCells count="18">
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C10:D10"/>
-    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B52:D52"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B64:D64"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B63:D63"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B28:B29"/>
     <mergeCell ref="B21:B24"/>
-    <mergeCell ref="B32:B39"/>
+    <mergeCell ref="B33:B40"/>
     <mergeCell ref="B17:B20"/>
   </mergeCells>
-  <conditionalFormatting sqref="F21:F39">
+  <conditionalFormatting sqref="F21:F40">
     <cfRule type="containsText" dxfId="57" priority="96" operator="containsText" text="NOT NEEDED">
       <formula>NOT(ISERROR(SEARCH(("NOT NEEDED"),(F21))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F21:F39">
+  <conditionalFormatting sqref="F21:F40">
     <cfRule type="containsText" dxfId="56" priority="97" operator="containsText" text="OPTIONAL">
       <formula>NOT(ISERROR(SEARCH(("OPTIONAL"),(F21))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F21:F39">
+  <conditionalFormatting sqref="F21:F40">
     <cfRule type="containsText" dxfId="55" priority="98" operator="containsText" text="REQUIRED">
       <formula>NOT(ISERROR(SEARCH(("REQUIRED"),(F21))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C62 C65:C979">
+  <conditionalFormatting sqref="C67 C70:C984">
     <cfRule type="containsText" dxfId="54" priority="99" operator="containsText" text="CONDITIONAL">
-      <formula>NOT(ISERROR(SEARCH(("CONDITIONAL"),(C62))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("CONDITIONAL"),(C67))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C62 C65:C979">
+  <conditionalFormatting sqref="C67 C70:C984">
     <cfRule type="containsText" dxfId="53" priority="100" operator="containsText" text="NOT NEEDED">
-      <formula>NOT(ISERROR(SEARCH(("NOT NEEDED"),(C62))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("NOT NEEDED"),(C67))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C62 C65:C979">
+  <conditionalFormatting sqref="C67 C70:C984">
     <cfRule type="containsText" dxfId="52" priority="101" operator="containsText" text="OPTIONAL">
-      <formula>NOT(ISERROR(SEARCH(("OPTIONAL"),(C62))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("OPTIONAL"),(C67))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C62 C65:C979">
+  <conditionalFormatting sqref="C67 C70:C984">
     <cfRule type="containsText" dxfId="51" priority="102" operator="containsText" text="REQUIRED">
-      <formula>NOT(ISERROR(SEARCH(("REQUIRED"),(C62))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("REQUIRED"),(C67))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C40">
+  <conditionalFormatting sqref="C41">
     <cfRule type="containsText" dxfId="50" priority="52" operator="containsText" text="CONDITIONAL">
-      <formula>NOT(ISERROR(SEARCH(("CONDITIONAL"),(C40))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("CONDITIONAL"),(C41))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C40">
+  <conditionalFormatting sqref="C41">
     <cfRule type="containsText" dxfId="49" priority="53" operator="containsText" text="NOT NEEDED">
-      <formula>NOT(ISERROR(SEARCH(("NOT NEEDED"),(C40))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("NOT NEEDED"),(C41))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C40">
+  <conditionalFormatting sqref="C41">
     <cfRule type="containsText" dxfId="48" priority="54" operator="containsText" text="OPTIONAL">
-      <formula>NOT(ISERROR(SEARCH(("OPTIONAL"),(C40))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("OPTIONAL"),(C41))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C40">
+  <conditionalFormatting sqref="C41">
     <cfRule type="containsText" dxfId="47" priority="55" operator="containsText" text="REQUIRED">
-      <formula>NOT(ISERROR(SEARCH(("REQUIRED"),(C40))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("REQUIRED"),(C41))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
@@ -9797,22 +10167,22 @@
       <formula>NOT(ISERROR(SEARCH(("REQUIRED"),(C24))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C25:C26">
+  <conditionalFormatting sqref="C25:C27">
     <cfRule type="containsText" dxfId="42" priority="25" operator="containsText" text="CONDITIONAL">
       <formula>NOT(ISERROR(SEARCH(("CONDITIONAL"),(C25))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C25:C26">
+  <conditionalFormatting sqref="C25:C27">
     <cfRule type="containsText" dxfId="41" priority="26" operator="containsText" text="NOT NEEDED">
       <formula>NOT(ISERROR(SEARCH(("NOT NEEDED"),(C25))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C25:C26">
+  <conditionalFormatting sqref="C25:C27">
     <cfRule type="containsText" dxfId="40" priority="27" operator="containsText" text="OPTIONAL">
       <formula>NOT(ISERROR(SEARCH(("OPTIONAL"),(C25))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C25:C26">
+  <conditionalFormatting sqref="C25:C27">
     <cfRule type="containsText" dxfId="39" priority="28" operator="containsText" text="REQUIRED">
       <formula>NOT(ISERROR(SEARCH(("REQUIRED"),(C25))))</formula>
     </cfRule>
@@ -9837,102 +10207,102 @@
       <formula>NOT(ISERROR(SEARCH(("REQUIRED"),(C22))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C29">
+  <conditionalFormatting sqref="C30">
     <cfRule type="containsText" dxfId="34" priority="21" operator="containsText" text="CONDITIONAL">
-      <formula>NOT(ISERROR(SEARCH(("CONDITIONAL"),(C29))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C29">
-    <cfRule type="containsText" dxfId="33" priority="22" operator="containsText" text="NOT NEEDED">
-      <formula>NOT(ISERROR(SEARCH(("NOT NEEDED"),(C29))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C29">
-    <cfRule type="containsText" dxfId="32" priority="23" operator="containsText" text="OPTIONAL">
-      <formula>NOT(ISERROR(SEARCH(("OPTIONAL"),(C29))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C29">
-    <cfRule type="containsText" dxfId="31" priority="24" operator="containsText" text="REQUIRED">
-      <formula>NOT(ISERROR(SEARCH(("REQUIRED"),(C29))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C30">
-    <cfRule type="containsText" dxfId="30" priority="17" operator="containsText" text="CONDITIONAL">
       <formula>NOT(ISERROR(SEARCH(("CONDITIONAL"),(C30))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="containsText" dxfId="29" priority="18" operator="containsText" text="NOT NEEDED">
+    <cfRule type="containsText" dxfId="33" priority="22" operator="containsText" text="NOT NEEDED">
       <formula>NOT(ISERROR(SEARCH(("NOT NEEDED"),(C30))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="containsText" dxfId="28" priority="19" operator="containsText" text="OPTIONAL">
+    <cfRule type="containsText" dxfId="32" priority="23" operator="containsText" text="OPTIONAL">
       <formula>NOT(ISERROR(SEARCH(("OPTIONAL"),(C30))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="containsText" dxfId="27" priority="20" operator="containsText" text="REQUIRED">
+    <cfRule type="containsText" dxfId="31" priority="24" operator="containsText" text="REQUIRED">
       <formula>NOT(ISERROR(SEARCH(("REQUIRED"),(C30))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
-    <cfRule type="containsText" dxfId="26" priority="13" operator="containsText" text="CONDITIONAL">
+    <cfRule type="containsText" dxfId="30" priority="17" operator="containsText" text="CONDITIONAL">
       <formula>NOT(ISERROR(SEARCH(("CONDITIONAL"),(C31))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
-    <cfRule type="containsText" dxfId="25" priority="14" operator="containsText" text="NOT NEEDED">
+    <cfRule type="containsText" dxfId="29" priority="18" operator="containsText" text="NOT NEEDED">
       <formula>NOT(ISERROR(SEARCH(("NOT NEEDED"),(C31))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
-    <cfRule type="containsText" dxfId="24" priority="15" operator="containsText" text="OPTIONAL">
+    <cfRule type="containsText" dxfId="28" priority="19" operator="containsText" text="OPTIONAL">
       <formula>NOT(ISERROR(SEARCH(("OPTIONAL"),(C31))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
-    <cfRule type="containsText" dxfId="23" priority="16" operator="containsText" text="REQUIRED">
+    <cfRule type="containsText" dxfId="27" priority="20" operator="containsText" text="REQUIRED">
       <formula>NOT(ISERROR(SEARCH(("REQUIRED"),(C31))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C41:C43">
-    <cfRule type="containsText" dxfId="22" priority="9" operator="containsText" text="CONDITIONAL">
-      <formula>NOT(ISERROR(SEARCH(("CONDITIONAL"),(C41))))</formula>
+  <conditionalFormatting sqref="C32">
+    <cfRule type="containsText" dxfId="26" priority="13" operator="containsText" text="CONDITIONAL">
+      <formula>NOT(ISERROR(SEARCH(("CONDITIONAL"),(C32))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C41:C43">
-    <cfRule type="containsText" dxfId="21" priority="10" operator="containsText" text="NOT NEEDED">
-      <formula>NOT(ISERROR(SEARCH(("NOT NEEDED"),(C41))))</formula>
+  <conditionalFormatting sqref="C32">
+    <cfRule type="containsText" dxfId="25" priority="14" operator="containsText" text="NOT NEEDED">
+      <formula>NOT(ISERROR(SEARCH(("NOT NEEDED"),(C32))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C41:C43">
-    <cfRule type="containsText" dxfId="20" priority="11" operator="containsText" text="OPTIONAL">
-      <formula>NOT(ISERROR(SEARCH(("OPTIONAL"),(C41))))</formula>
+  <conditionalFormatting sqref="C32">
+    <cfRule type="containsText" dxfId="24" priority="15" operator="containsText" text="OPTIONAL">
+      <formula>NOT(ISERROR(SEARCH(("OPTIONAL"),(C32))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C41:C43">
-    <cfRule type="containsText" dxfId="19" priority="12" operator="containsText" text="REQUIRED">
-      <formula>NOT(ISERROR(SEARCH(("REQUIRED"),(C41))))</formula>
+  <conditionalFormatting sqref="C32">
+    <cfRule type="containsText" dxfId="23" priority="16" operator="containsText" text="REQUIRED">
+      <formula>NOT(ISERROR(SEARCH(("REQUIRED"),(C32))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C32:C39 C21 C44:C47 C50">
+  <conditionalFormatting sqref="C42:C44">
+    <cfRule type="containsText" dxfId="22" priority="9" operator="containsText" text="CONDITIONAL">
+      <formula>NOT(ISERROR(SEARCH(("CONDITIONAL"),(C42))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C42:C44">
+    <cfRule type="containsText" dxfId="21" priority="10" operator="containsText" text="NOT NEEDED">
+      <formula>NOT(ISERROR(SEARCH(("NOT NEEDED"),(C42))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C42:C44">
+    <cfRule type="containsText" dxfId="20" priority="11" operator="containsText" text="OPTIONAL">
+      <formula>NOT(ISERROR(SEARCH(("OPTIONAL"),(C42))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C42:C44">
+    <cfRule type="containsText" dxfId="19" priority="12" operator="containsText" text="REQUIRED">
+      <formula>NOT(ISERROR(SEARCH(("REQUIRED"),(C42))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C33:C40 C21 C45:C48 C51">
     <cfRule type="containsText" dxfId="18" priority="45" operator="containsText" text="NOT NEEDED">
       <formula>NOT(ISERROR(SEARCH(("NOT NEEDED"),(C21))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C32:C39 C21 C44:C47 C50">
+  <conditionalFormatting sqref="C33:C40 C21 C45:C48 C51">
     <cfRule type="containsText" dxfId="17" priority="46" operator="containsText" text="OPTIONAL">
       <formula>NOT(ISERROR(SEARCH(("OPTIONAL"),(C21))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C32:C39 C21 C44:C47 C50">
+  <conditionalFormatting sqref="C33:C40 C21 C45:C48 C51">
     <cfRule type="containsText" dxfId="16" priority="47" operator="containsText" text="REQUIRED">
       <formula>NOT(ISERROR(SEARCH(("REQUIRED"),(C21))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C16:C17 C32:C39 C21 C44:C47 C50">
+  <conditionalFormatting sqref="C16:C17 C33:C40 C21 C45:C48 C51">
     <cfRule type="containsText" dxfId="15" priority="48" operator="containsText" text="CONDITIONAL">
       <formula>NOT(ISERROR(SEARCH(("CONDITIONAL"),(C16))))</formula>
     </cfRule>
@@ -9952,69 +10322,69 @@
       <formula>NOT(ISERROR(SEARCH(("REQUIRED"),(C16))))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C29">
+    <cfRule type="containsText" dxfId="11" priority="41" operator="containsText" text="CONDITIONAL">
+      <formula>NOT(ISERROR(SEARCH(("CONDITIONAL"),(C29))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C29">
+    <cfRule type="containsText" dxfId="10" priority="42" operator="containsText" text="NOT NEEDED">
+      <formula>NOT(ISERROR(SEARCH(("NOT NEEDED"),(C29))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C29">
+    <cfRule type="containsText" dxfId="9" priority="43" operator="containsText" text="OPTIONAL">
+      <formula>NOT(ISERROR(SEARCH(("OPTIONAL"),(C29))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C29">
+    <cfRule type="containsText" dxfId="8" priority="44" operator="containsText" text="REQUIRED">
+      <formula>NOT(ISERROR(SEARCH(("REQUIRED"),(C29))))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="containsText" dxfId="11" priority="41" operator="containsText" text="CONDITIONAL">
+    <cfRule type="containsText" dxfId="7" priority="37" operator="containsText" text="CONDITIONAL">
       <formula>NOT(ISERROR(SEARCH(("CONDITIONAL"),(C28))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="containsText" dxfId="10" priority="42" operator="containsText" text="NOT NEEDED">
+    <cfRule type="containsText" dxfId="6" priority="38" operator="containsText" text="NOT NEEDED">
       <formula>NOT(ISERROR(SEARCH(("NOT NEEDED"),(C28))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="containsText" dxfId="9" priority="43" operator="containsText" text="OPTIONAL">
+    <cfRule type="containsText" dxfId="5" priority="39" operator="containsText" text="OPTIONAL">
       <formula>NOT(ISERROR(SEARCH(("OPTIONAL"),(C28))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="containsText" dxfId="8" priority="44" operator="containsText" text="REQUIRED">
+    <cfRule type="containsText" dxfId="4" priority="40" operator="containsText" text="REQUIRED">
       <formula>NOT(ISERROR(SEARCH(("REQUIRED"),(C28))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C27">
-    <cfRule type="containsText" dxfId="7" priority="37" operator="containsText" text="CONDITIONAL">
-      <formula>NOT(ISERROR(SEARCH(("CONDITIONAL"),(C27))))</formula>
+  <conditionalFormatting sqref="C49:C50">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="NOT NEEDED">
+      <formula>NOT(ISERROR(SEARCH(("NOT NEEDED"),(C49))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C27">
-    <cfRule type="containsText" dxfId="6" priority="38" operator="containsText" text="NOT NEEDED">
-      <formula>NOT(ISERROR(SEARCH(("NOT NEEDED"),(C27))))</formula>
+  <conditionalFormatting sqref="C49:C50">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="OPTIONAL">
+      <formula>NOT(ISERROR(SEARCH(("OPTIONAL"),(C49))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C27">
-    <cfRule type="containsText" dxfId="5" priority="39" operator="containsText" text="OPTIONAL">
-      <formula>NOT(ISERROR(SEARCH(("OPTIONAL"),(C27))))</formula>
+  <conditionalFormatting sqref="C49:C50">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="REQUIRED">
+      <formula>NOT(ISERROR(SEARCH(("REQUIRED"),(C49))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C27">
-    <cfRule type="containsText" dxfId="4" priority="40" operator="containsText" text="REQUIRED">
-      <formula>NOT(ISERROR(SEARCH(("REQUIRED"),(C27))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48:C49">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="NOT NEEDED">
-      <formula>NOT(ISERROR(SEARCH(("NOT NEEDED"),(C48))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48:C49">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="OPTIONAL">
-      <formula>NOT(ISERROR(SEARCH(("OPTIONAL"),(C48))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48:C49">
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="REQUIRED">
-      <formula>NOT(ISERROR(SEARCH(("REQUIRED"),(C48))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48:C49">
+  <conditionalFormatting sqref="C49:C50">
     <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="CONDITIONAL">
-      <formula>NOT(ISERROR(SEARCH(("CONDITIONAL"),(C48))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("CONDITIONAL"),(C49))))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="C11" r:id="rId1" xr:uid="{9E0D5031-4E1D-8441-819B-76A236A6B1A5}"/>
-    <hyperlink ref="B63" r:id="rId2" display="https://creativecommons.org/licenses/by-nc-sa/3.0/igo" xr:uid="{437BAFF1-5BC7-374A-8547-8511AAB89284}"/>
+    <hyperlink ref="B68" r:id="rId2" display="https://creativecommons.org/licenses/by-nc-sa/3.0/igo" xr:uid="{437BAFF1-5BC7-374A-8547-8511AAB89284}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -10024,7 +10394,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6701640C-B18C-FC4B-AB3F-FF97B6506D59}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView zoomScale="101" workbookViewId="0"/>
   </sheetViews>
@@ -10068,7 +10438,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>15</v>
@@ -10077,7 +10447,7 @@
         <v>14</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14" x14ac:dyDescent="0.15">
@@ -10175,7 +10545,7 @@
         <v>30</v>
       </c>
       <c r="C9" s="35" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="35" t="s">
@@ -10202,7 +10572,7 @@
         <v>165</v>
       </c>
       <c r="G10" s="131" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="42" x14ac:dyDescent="0.15">
@@ -10223,7 +10593,7 @@
         <v>166</v>
       </c>
       <c r="G11" s="31" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="28" x14ac:dyDescent="0.15">
@@ -10244,7 +10614,7 @@
         <v>48</v>
       </c>
       <c r="G12" s="30" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="14" x14ac:dyDescent="0.15">
@@ -10262,13 +10632,13 @@
         <v>1</v>
       </c>
       <c r="F13" s="127" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G13" s="30" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="56" x14ac:dyDescent="0.15">
       <c r="A14" s="39" t="s">
         <v>4</v>
       </c>
@@ -10283,10 +10653,10 @@
         <v>1</v>
       </c>
       <c r="F14" s="127" t="s">
-        <v>208</v>
+        <v>306</v>
       </c>
       <c r="G14" s="30" t="s">
-        <v>209</v>
+        <v>307</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="14" x14ac:dyDescent="0.15">
@@ -10321,7 +10691,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="127"/>
-      <c r="G16" s="30"/>
+      <c r="G16" s="135"/>
     </row>
     <row r="17" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A17" s="39" t="s">
@@ -10357,10 +10727,10 @@
         <v>1</v>
       </c>
       <c r="F18" s="127" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="G18" s="30" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="14" x14ac:dyDescent="0.15">
@@ -10378,10 +10748,10 @@
         <v>1</v>
       </c>
       <c r="F19" s="127" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G19" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="14" x14ac:dyDescent="0.15">
@@ -10402,6 +10772,263 @@
       </c>
       <c r="F20" s="129"/>
       <c r="G20" s="33"/>
+    </row>
+    <row r="21" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A21" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="51" t="s">
+        <v>225</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="29"/>
+      <c r="E21" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" s="126"/>
+      <c r="G21" s="136"/>
+    </row>
+    <row r="22" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A22" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="50" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="35" t="s">
+        <v>226</v>
+      </c>
+      <c r="D22" s="25"/>
+      <c r="E22" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" s="127"/>
+      <c r="G22" s="137"/>
+    </row>
+    <row r="23" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A23" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="25"/>
+      <c r="E23" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="F23" s="127" t="s">
+        <v>165</v>
+      </c>
+      <c r="G23" s="131" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A24" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="48" t="s">
+        <v>227</v>
+      </c>
+      <c r="C24" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="25"/>
+      <c r="E24" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="F24" s="127" t="s">
+        <v>228</v>
+      </c>
+      <c r="G24" s="137" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="409.6" x14ac:dyDescent="0.15">
+      <c r="A25" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="48" t="s">
+        <v>229</v>
+      </c>
+      <c r="C25" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" s="25"/>
+      <c r="E25" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" s="127" t="s">
+        <v>297</v>
+      </c>
+      <c r="G25" s="148" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="409.6" x14ac:dyDescent="0.15">
+      <c r="A26" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="48" t="s">
+        <v>230</v>
+      </c>
+      <c r="C26" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="25"/>
+      <c r="E26" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="F26" s="127" t="s">
+        <v>298</v>
+      </c>
+      <c r="G26" s="148" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="28" x14ac:dyDescent="0.15">
+      <c r="A27" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="48" t="s">
+        <v>231</v>
+      </c>
+      <c r="C27" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="E27" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="F27" s="127" t="s">
+        <v>232</v>
+      </c>
+      <c r="G27" s="137"/>
+    </row>
+    <row r="28" spans="1:7" ht="28" x14ac:dyDescent="0.15">
+      <c r="A28" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="48" t="s">
+        <v>233</v>
+      </c>
+      <c r="C28" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="F28" s="127" t="s">
+        <v>232</v>
+      </c>
+      <c r="G28" s="137"/>
+    </row>
+    <row r="29" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A29" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="48" t="s">
+        <v>234</v>
+      </c>
+      <c r="C29" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="25"/>
+      <c r="E29" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="F29" s="127" t="s">
+        <v>48</v>
+      </c>
+      <c r="G29" s="137" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A30" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="48" t="s">
+        <v>235</v>
+      </c>
+      <c r="C30" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30" s="25"/>
+      <c r="E30" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="F30" s="127"/>
+      <c r="G30" s="137"/>
+    </row>
+    <row r="31" spans="1:7" ht="42" x14ac:dyDescent="0.15">
+      <c r="A31" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="48" t="s">
+        <v>236</v>
+      </c>
+      <c r="C31" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="D31" s="30"/>
+      <c r="E31" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="F31" s="127" t="s">
+        <v>217</v>
+      </c>
+      <c r="G31" s="30" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A32" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="48" t="s">
+        <v>237</v>
+      </c>
+      <c r="C32" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="D32" s="25"/>
+      <c r="E32" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="F32" s="127" t="s">
+        <v>191</v>
+      </c>
+      <c r="G32" s="30" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A33" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="52" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33" s="33"/>
+      <c r="E33" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="F33" s="129"/>
+      <c r="G33" s="138"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10410,7 +11037,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CEF3E87-3882-C14D-A464-A5139BF1245B}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -10589,7 +11216,7 @@
         <v>56</v>
       </c>
       <c r="E10" s="67" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F10" s="63" t="s">
         <v>72</v>
@@ -10609,7 +11236,7 @@
         <v>57</v>
       </c>
       <c r="E11" s="67" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F11" s="63" t="s">
         <v>161</v>
@@ -10629,7 +11256,7 @@
         <v>58</v>
       </c>
       <c r="E12" s="72" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F12" s="63" t="s">
         <v>73</v>
@@ -10649,13 +11276,13 @@
         <v>59</v>
       </c>
       <c r="E13" s="72" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="F13" s="63" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="42" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6" ht="56" x14ac:dyDescent="0.15">
       <c r="A14" s="57" t="s">
         <v>25</v>
       </c>
@@ -10669,7 +11296,7 @@
         <v>60</v>
       </c>
       <c r="E14" s="72" t="s">
-        <v>207</v>
+        <v>305</v>
       </c>
       <c r="F14" s="63" t="s">
         <v>162</v>
@@ -10743,7 +11370,7 @@
         <v>81</v>
       </c>
       <c r="E18" s="67" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="F18" s="63" t="s">
         <v>99</v>
@@ -10763,7 +11390,7 @@
         <v>64</v>
       </c>
       <c r="E19" s="67" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F19" s="63" t="s">
         <v>78</v>
@@ -10784,6 +11411,254 @@
       </c>
       <c r="E20" s="69"/>
       <c r="F20" s="75" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="28" x14ac:dyDescent="0.15">
+      <c r="A21" s="139" t="s">
+        <v>238</v>
+      </c>
+      <c r="B21" s="140" t="s">
+        <v>239</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>225</v>
+      </c>
+      <c r="D21" s="71" t="s">
+        <v>240</v>
+      </c>
+      <c r="E21" s="65"/>
+      <c r="F21" s="71" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="28" x14ac:dyDescent="0.15">
+      <c r="A22" s="141" t="s">
+        <v>238</v>
+      </c>
+      <c r="B22" s="142" t="s">
+        <v>239</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="67"/>
+      <c r="F22" s="68" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="28" x14ac:dyDescent="0.15">
+      <c r="A23" s="141" t="s">
+        <v>238</v>
+      </c>
+      <c r="B23" s="142" t="s">
+        <v>239</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="63" t="s">
+        <v>242</v>
+      </c>
+      <c r="E23" s="67" t="s">
+        <v>199</v>
+      </c>
+      <c r="F23" s="68" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="28" x14ac:dyDescent="0.15">
+      <c r="A24" s="141" t="s">
+        <v>238</v>
+      </c>
+      <c r="B24" s="142" t="s">
+        <v>239</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="D24" s="63" t="s">
+        <v>268</v>
+      </c>
+      <c r="E24" s="67" t="s">
+        <v>263</v>
+      </c>
+      <c r="F24" s="68" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="409.6" x14ac:dyDescent="0.15">
+      <c r="A25" s="141" t="s">
+        <v>238</v>
+      </c>
+      <c r="B25" s="142" t="s">
+        <v>239</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="D25" s="63" t="s">
+        <v>264</v>
+      </c>
+      <c r="E25" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="F25" s="68" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="409.6" x14ac:dyDescent="0.15">
+      <c r="A26" s="141" t="s">
+        <v>238</v>
+      </c>
+      <c r="B26" s="142" t="s">
+        <v>239</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="D26" s="63" t="s">
+        <v>246</v>
+      </c>
+      <c r="E26" s="67" t="s">
+        <v>266</v>
+      </c>
+      <c r="F26" s="68" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="28" x14ac:dyDescent="0.15">
+      <c r="A27" s="141" t="s">
+        <v>238</v>
+      </c>
+      <c r="B27" s="142" t="s">
+        <v>239</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="D27" s="63" t="s">
+        <v>248</v>
+      </c>
+      <c r="E27" s="67"/>
+      <c r="F27" s="68" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="28" x14ac:dyDescent="0.15">
+      <c r="A28" s="141" t="s">
+        <v>238</v>
+      </c>
+      <c r="B28" s="142" t="s">
+        <v>239</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="D28" s="63" t="s">
+        <v>250</v>
+      </c>
+      <c r="E28" s="67"/>
+      <c r="F28" s="68" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="28" x14ac:dyDescent="0.15">
+      <c r="A29" s="141" t="s">
+        <v>238</v>
+      </c>
+      <c r="B29" s="142" t="s">
+        <v>239</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="D29" s="63" t="s">
+        <v>252</v>
+      </c>
+      <c r="E29" s="67" t="s">
+        <v>262</v>
+      </c>
+      <c r="F29" s="68" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="28" x14ac:dyDescent="0.15">
+      <c r="A30" s="141" t="s">
+        <v>238</v>
+      </c>
+      <c r="B30" s="142" t="s">
+        <v>239</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="D30" s="63" t="s">
+        <v>254</v>
+      </c>
+      <c r="E30" s="67"/>
+      <c r="F30" s="68" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="70" x14ac:dyDescent="0.15">
+      <c r="A31" s="141" t="s">
+        <v>238</v>
+      </c>
+      <c r="B31" s="142" t="s">
+        <v>239</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="D31" s="63" t="s">
+        <v>256</v>
+      </c>
+      <c r="E31" s="67" t="s">
+        <v>219</v>
+      </c>
+      <c r="F31" s="63" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="28" x14ac:dyDescent="0.15">
+      <c r="A32" s="141" t="s">
+        <v>238</v>
+      </c>
+      <c r="B32" s="142" t="s">
+        <v>239</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="D32" s="63" t="s">
+        <v>258</v>
+      </c>
+      <c r="E32" s="67" t="s">
+        <v>190</v>
+      </c>
+      <c r="F32" s="68" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="42" x14ac:dyDescent="0.15">
+      <c r="A33" s="143" t="s">
+        <v>238</v>
+      </c>
+      <c r="B33" s="144" t="s">
+        <v>239</v>
+      </c>
+      <c r="C33" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" s="64" t="s">
+        <v>65</v>
+      </c>
+      <c r="E33" s="69"/>
+      <c r="F33" s="75" t="s">
         <v>79</v>
       </c>
     </row>
@@ -10795,7 +11670,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D1882CD-2CE8-9D4B-9D63-04C5D805B201}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -10975,7 +11850,7 @@
         <v>88</v>
       </c>
       <c r="E10" s="67" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F10" s="63" t="s">
         <v>106</v>
@@ -10995,7 +11870,7 @@
         <v>89</v>
       </c>
       <c r="E11" s="67" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F11" s="63" t="s">
         <v>163</v>
@@ -11015,7 +11890,7 @@
         <v>90</v>
       </c>
       <c r="E12" s="72" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F12" s="63" t="s">
         <v>107</v>
@@ -11035,7 +11910,7 @@
         <v>91</v>
       </c>
       <c r="E13" s="72" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="F13" s="63" t="s">
         <v>108</v>
@@ -11055,7 +11930,7 @@
         <v>92</v>
       </c>
       <c r="E14" s="72" t="s">
-        <v>207</v>
+        <v>305</v>
       </c>
       <c r="F14" s="63" t="s">
         <v>164</v>
@@ -11129,7 +12004,7 @@
         <v>96</v>
       </c>
       <c r="E18" s="67" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="F18" s="63" t="s">
         <v>112</v>
@@ -11149,7 +12024,7 @@
         <v>97</v>
       </c>
       <c r="E19" s="67" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F19" s="63" t="s">
         <v>113</v>
@@ -11172,6 +12047,257 @@
       <c r="F20" s="75" t="s">
         <v>114</v>
       </c>
+    </row>
+    <row r="21" spans="1:6" ht="42" x14ac:dyDescent="0.15">
+      <c r="A21" s="139" t="s">
+        <v>270</v>
+      </c>
+      <c r="B21" s="140" t="s">
+        <v>271</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>225</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>272</v>
+      </c>
+      <c r="E21" s="65"/>
+      <c r="F21" s="71" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="42" x14ac:dyDescent="0.15">
+      <c r="A22" s="141" t="s">
+        <v>270</v>
+      </c>
+      <c r="B22" s="142" t="s">
+        <v>271</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="62" t="s">
+        <v>86</v>
+      </c>
+      <c r="E22" s="67"/>
+      <c r="F22" s="68" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="42" x14ac:dyDescent="0.15">
+      <c r="A23" s="141" t="s">
+        <v>270</v>
+      </c>
+      <c r="B23" s="142" t="s">
+        <v>271</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="180" t="s">
+        <v>274</v>
+      </c>
+      <c r="E23" s="67" t="s">
+        <v>199</v>
+      </c>
+      <c r="F23" s="68" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="42" x14ac:dyDescent="0.15">
+      <c r="A24" s="141" t="s">
+        <v>270</v>
+      </c>
+      <c r="B24" s="142" t="s">
+        <v>271</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="D24" s="180" t="s">
+        <v>293</v>
+      </c>
+      <c r="E24" s="67" t="s">
+        <v>296</v>
+      </c>
+      <c r="F24" s="68" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="409.6" x14ac:dyDescent="0.15">
+      <c r="A25" s="141" t="s">
+        <v>270</v>
+      </c>
+      <c r="B25" s="142" t="s">
+        <v>271</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="D25" s="180" t="s">
+        <v>277</v>
+      </c>
+      <c r="E25" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="F25" s="68" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="409.6" x14ac:dyDescent="0.15">
+      <c r="A26" s="141" t="s">
+        <v>270</v>
+      </c>
+      <c r="B26" s="142" t="s">
+        <v>271</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="D26" s="180" t="s">
+        <v>279</v>
+      </c>
+      <c r="E26" s="67" t="s">
+        <v>294</v>
+      </c>
+      <c r="F26" s="68" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="42" x14ac:dyDescent="0.15">
+      <c r="A27" s="141" t="s">
+        <v>270</v>
+      </c>
+      <c r="B27" s="142" t="s">
+        <v>271</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="D27" s="180" t="s">
+        <v>281</v>
+      </c>
+      <c r="E27" s="67"/>
+      <c r="F27" s="68" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="42" x14ac:dyDescent="0.15">
+      <c r="A28" s="141" t="s">
+        <v>270</v>
+      </c>
+      <c r="B28" s="142" t="s">
+        <v>271</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="D28" s="180" t="s">
+        <v>283</v>
+      </c>
+      <c r="E28" s="67"/>
+      <c r="F28" s="68" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="42" x14ac:dyDescent="0.15">
+      <c r="A29" s="141" t="s">
+        <v>270</v>
+      </c>
+      <c r="B29" s="142" t="s">
+        <v>271</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="D29" s="180" t="s">
+        <v>285</v>
+      </c>
+      <c r="E29" s="67" t="s">
+        <v>295</v>
+      </c>
+      <c r="F29" s="68" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="42" x14ac:dyDescent="0.15">
+      <c r="A30" s="141" t="s">
+        <v>270</v>
+      </c>
+      <c r="B30" s="142" t="s">
+        <v>271</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="D30" s="180" t="s">
+        <v>287</v>
+      </c>
+      <c r="E30" s="67"/>
+      <c r="F30" s="68" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="70" x14ac:dyDescent="0.15">
+      <c r="A31" s="141" t="s">
+        <v>270</v>
+      </c>
+      <c r="B31" s="142" t="s">
+        <v>271</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="D31" s="30" t="s">
+        <v>289</v>
+      </c>
+      <c r="E31" s="67" t="s">
+        <v>220</v>
+      </c>
+      <c r="F31" s="63" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="42" x14ac:dyDescent="0.15">
+      <c r="A32" s="141" t="s">
+        <v>270</v>
+      </c>
+      <c r="B32" s="142" t="s">
+        <v>271</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="D32" s="180" t="s">
+        <v>291</v>
+      </c>
+      <c r="E32" s="67" t="s">
+        <v>194</v>
+      </c>
+      <c r="F32" s="68" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="42" x14ac:dyDescent="0.15">
+      <c r="A33" s="143" t="s">
+        <v>270</v>
+      </c>
+      <c r="B33" s="144" t="s">
+        <v>271</v>
+      </c>
+      <c r="C33" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" s="64" t="s">
+        <v>98</v>
+      </c>
+      <c r="E33" s="69"/>
+      <c r="F33" s="75" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="E37" s="181"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>